<commit_message>
Latest adjustments by Loes Segers
</commit_message>
<xml_diff>
--- a/notebooks/Data Zuid_Beveland.xlsx
+++ b/notebooks/Data Zuid_Beveland.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K150"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,16 +513,16 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1.028666236678933</v>
+        <v>1.037421013340637</v>
       </c>
       <c r="F2" t="n">
-        <v>797.2325658953798</v>
+        <v>803.6279822723031</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3790779410622814</v>
+        <v>0.3798188787296788</v>
       </c>
       <c r="H2" t="n">
-        <v>11.3587543753095</v>
+        <v>11.39099227506674</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -552,16 +552,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.08451783701297903</v>
+        <v>0.08523715166908165</v>
       </c>
       <c r="F3" t="n">
-        <v>65.50265742816515</v>
+        <v>66.0281210597506</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03114600904722796</v>
+        <v>0.03120688637008513</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9332641860830024</v>
+        <v>0.9359129338193811</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -591,16 +591,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1.411556705765194</v>
+        <v>1.423570188035951</v>
       </c>
       <c r="F4" t="n">
-        <v>1093.97872154419</v>
+        <v>1102.754641734423</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5201784514518717</v>
+        <v>0.5211951811671995</v>
       </c>
       <c r="H4" t="n">
-        <v>15.58671349829465</v>
+        <v>15.63095099897497</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -632,16 +632,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>12.55436370851586</v>
+        <v>12.66121143538154</v>
       </c>
       <c r="F5" t="n">
-        <v>9729.829984008669</v>
+        <v>9807.882883441504</v>
       </c>
       <c r="G5" t="n">
-        <v>4.626459176394394</v>
+        <v>4.63550195489137</v>
       </c>
       <c r="H5" t="n">
-        <v>138.6279910105275</v>
+        <v>139.0214386628737</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.5864949038686279</v>
+        <v>0.5914864470464367</v>
       </c>
       <c r="F6" t="n">
-        <v>454.5428054347958</v>
+        <v>458.189157388254</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2161316008528406</v>
+        <v>0.216554047076514</v>
       </c>
       <c r="H6" t="n">
-        <v>6.476203179052959</v>
+        <v>6.49458364429206</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -712,16 +712,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3.770444480407066</v>
+        <v>3.802533993780668</v>
       </c>
       <c r="F7" t="n">
-        <v>2922.153970540275</v>
+        <v>2945.595550755997</v>
       </c>
       <c r="G7" t="n">
-        <v>1.38946169396546</v>
+        <v>1.392177506177558</v>
       </c>
       <c r="H7" t="n">
-        <v>41.63406092587326</v>
+        <v>41.75222482201474</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -749,16 +749,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>5.754671696648729</v>
+        <v>5.803648578588181</v>
       </c>
       <c r="F8" t="n">
-        <v>4459.961374580253</v>
+        <v>4495.739277889275</v>
       </c>
       <c r="G8" t="n">
-        <v>2.12067726391665</v>
+        <v>2.124822294494928</v>
       </c>
       <c r="H8" t="n">
-        <v>63.54432568566668</v>
+        <v>63.72467429756008</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -790,16 +790,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>5.08114944786374</v>
+        <v>5.12439411429237</v>
       </c>
       <c r="F9" t="n">
-        <v>3937.971003365529</v>
+        <v>3969.561489177351</v>
       </c>
       <c r="G9" t="n">
-        <v>1.872474864338489</v>
+        <v>1.87613476380463</v>
       </c>
       <c r="H9" t="n">
-        <v>56.10714777230029</v>
+        <v>56.26638852501881</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -831,16 +831,16 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3.3326667082876</v>
+        <v>3.361030380767589</v>
       </c>
       <c r="F10" t="n">
-        <v>2582.869289017601</v>
+        <v>2603.589120320543</v>
       </c>
       <c r="G10" t="n">
-        <v>1.228134442971894</v>
+        <v>1.230534928372681</v>
       </c>
       <c r="H10" t="n">
-        <v>36.80002438590079</v>
+        <v>36.90446853926365</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -872,16 +872,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>3.060202148439766</v>
+        <v>3.086246928848442</v>
       </c>
       <c r="F11" t="n">
-        <v>2371.704955424908</v>
+        <v>2390.730822286288</v>
       </c>
       <c r="G11" t="n">
-        <v>1.127727428609341</v>
+        <v>1.129931660611883</v>
       </c>
       <c r="H11" t="n">
-        <v>33.79141193892032</v>
+        <v>33.88731718627587</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -913,16 +913,16 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>9.154442822582761</v>
+        <v>9.232354489770803</v>
       </c>
       <c r="F12" t="n">
-        <v>7094.837646076003</v>
+        <v>7151.752581957268</v>
       </c>
       <c r="G12" t="n">
-        <v>3.373540625587783</v>
+        <v>3.380134476192187</v>
       </c>
       <c r="H12" t="n">
-        <v>101.0853315008453</v>
+        <v>101.3722272864267</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -954,16 +954,16 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>6.369028161182413</v>
+        <v>6.423233710400618</v>
       </c>
       <c r="F13" t="n">
-        <v>4936.097329278657</v>
+        <v>4975.694805107594</v>
       </c>
       <c r="G13" t="n">
-        <v>2.3470762413617</v>
+        <v>2.351663786553094</v>
       </c>
       <c r="H13" t="n">
-        <v>70.32818223961108</v>
+        <v>70.52778448411345</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -991,16 +991,16 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>9.422066807498156</v>
+        <v>9.502256170007097</v>
       </c>
       <c r="F14" t="n">
-        <v>7302.250457494509</v>
+        <v>7360.829263342477</v>
       </c>
       <c r="G14" t="n">
-        <v>3.472163818789063</v>
+        <v>3.478950436187622</v>
       </c>
       <c r="H14" t="n">
-        <v>104.0404932399119</v>
+        <v>104.3357762311933</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1032,16 +1032,16 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>11.50107238407059</v>
+        <v>11.5989557551281</v>
       </c>
       <c r="F15" t="n">
-        <v>8913.512586434004</v>
+        <v>8985.016970676666</v>
       </c>
       <c r="G15" t="n">
-        <v>4.238306544514302</v>
+        <v>4.246590648151559</v>
       </c>
       <c r="H15" t="n">
-        <v>126.9973210945173</v>
+        <v>127.3577591091533</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1073,16 +1073,16 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>7.588656398089183</v>
+        <v>7.653241964117739</v>
       </c>
       <c r="F16" t="n">
-        <v>5881.328458750302</v>
+        <v>5928.508598542753</v>
       </c>
       <c r="G16" t="n">
-        <v>2.796526358813038</v>
+        <v>2.801992389628681</v>
       </c>
       <c r="H16" t="n">
-        <v>83.7955801942352</v>
+        <v>84.03340499475287</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1110,16 +1110,16 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>7.751820568457165</v>
+        <v>7.817794792812919</v>
       </c>
       <c r="F17" t="n">
-        <v>6007.783265503068</v>
+        <v>6055.977828455124</v>
       </c>
       <c r="G17" t="n">
-        <v>2.856654644691003</v>
+        <v>2.862238200975337</v>
       </c>
       <c r="H17" t="n">
-        <v>85.59727413793745</v>
+        <v>85.84021242436886</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>4.6511732868204</v>
+        <v>4.690758510282906</v>
       </c>
       <c r="F18" t="n">
-        <v>3604.732693564538</v>
+        <v>3633.649934544672</v>
       </c>
       <c r="G18" t="n">
-        <v>1.71402261666272</v>
+        <v>1.717372808735919</v>
       </c>
       <c r="H18" t="n">
-        <v>51.35925830845731</v>
+        <v>51.50502381697446</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1192,16 +1192,16 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>5.257700018298514</v>
+        <v>5.302447271916499</v>
       </c>
       <c r="F19" t="n">
-        <v>4074.800481491042</v>
+        <v>4107.488616174768</v>
       </c>
       <c r="G19" t="n">
-        <v>1.937536226984354</v>
+        <v>1.941323294000352</v>
       </c>
       <c r="H19" t="n">
-        <v>58.05665724534379</v>
+        <v>58.22143100688338</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -1233,16 +1233,16 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>4.00029971433398</v>
+        <v>4.034345480561142</v>
       </c>
       <c r="F20" t="n">
-        <v>3100.295403963822</v>
+        <v>3125.166038513964</v>
       </c>
       <c r="G20" t="n">
-        <v>1.474166572611461</v>
+        <v>1.477047947175505</v>
       </c>
       <c r="H20" t="n">
-        <v>44.17217197592453</v>
+        <v>44.29753942340002</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1274,16 +1274,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>14.66775066825607</v>
+        <v>14.79258501699257</v>
       </c>
       <c r="F21" t="n">
-        <v>11367.73822738991</v>
+        <v>11458.93046098722</v>
       </c>
       <c r="G21" t="n">
-        <v>5.405271923856537</v>
+        <v>5.415836953150535</v>
       </c>
       <c r="H21" t="n">
-        <v>161.9644655018557</v>
+        <v>162.4241456736347</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -1311,16 +1311,16 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>4.260555698181841</v>
+        <v>4.296816452011061</v>
       </c>
       <c r="F22" t="n">
-        <v>3301.997898340215</v>
+        <v>3328.486594496752</v>
       </c>
       <c r="G22" t="n">
-        <v>1.570074554380347</v>
+        <v>1.573143388640513</v>
       </c>
       <c r="H22" t="n">
-        <v>47.04597466737737</v>
+        <v>47.1794984107468</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1348,16 +1348,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>3.778925404924198</v>
+        <v>3.811087097771572</v>
       </c>
       <c r="F23" t="n">
-        <v>2928.726820877012</v>
+        <v>2952.22112862736</v>
       </c>
       <c r="G23" t="n">
-        <v>1.392587033681185</v>
+        <v>1.395308954615297</v>
       </c>
       <c r="H23" t="n">
-        <v>41.72770912395124</v>
+        <v>41.8461388081174</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1389,16 +1389,16 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>7.251961719217994</v>
+        <v>7.313681742966353</v>
       </c>
       <c r="F24" t="n">
-        <v>5620.384769485254</v>
+        <v>5665.471613612373</v>
       </c>
       <c r="G24" t="n">
-        <v>2.672449645225125</v>
+        <v>2.677673158343901</v>
       </c>
       <c r="H24" t="n">
-        <v>80.07772494576913</v>
+        <v>80.30499789900438</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>4.79046960503888</v>
+        <v>4.831240352141075</v>
       </c>
       <c r="F25" t="n">
-        <v>3712.689538302688</v>
+        <v>3742.472811346757</v>
       </c>
       <c r="G25" t="n">
-        <v>1.765355264388837</v>
+        <v>1.768805790161156</v>
       </c>
       <c r="H25" t="n">
-        <v>52.89739828898698</v>
+        <v>53.04752927636435</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -1471,16 +1471,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3.436121138632219</v>
+        <v>3.465365291572847</v>
       </c>
       <c r="F26" t="n">
-        <v>2663.048105013746</v>
+        <v>2684.411132524694</v>
       </c>
       <c r="G26" t="n">
-        <v>1.26625885180829</v>
+        <v>1.268733854369314</v>
       </c>
       <c r="H26" t="n">
-        <v>37.94239050429798</v>
+        <v>38.05007686940433</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1510,16 +1510,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>4.006746532679776</v>
+        <v>4.040847166590261</v>
       </c>
       <c r="F27" t="n">
-        <v>3105.291789875198</v>
+        <v>3130.202505593379</v>
       </c>
       <c r="G27" t="n">
-        <v>1.476542315381639</v>
+        <v>1.479428333524483</v>
       </c>
       <c r="H27" t="n">
-        <v>44.24335912778596</v>
+        <v>44.36892861558277</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
@@ -1551,16 +1551,16 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>3.149913406174917</v>
+        <v>3.176721701350832</v>
       </c>
       <c r="F28" t="n">
-        <v>2441.2325959027</v>
+        <v>2460.816214840175</v>
       </c>
       <c r="G28" t="n">
-        <v>1.160787286296835</v>
+        <v>1.163056136387482</v>
       </c>
       <c r="H28" t="n">
-        <v>34.78202300251455</v>
+        <v>34.88073975672274</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2.047230285695695</v>
+        <v>2.06465386101451</v>
       </c>
       <c r="F29" t="n">
-        <v>1586.635777071823</v>
+        <v>1599.363802384759</v>
       </c>
       <c r="G29" t="n">
-        <v>0.7544330850785602</v>
+        <v>0.7559076839045196</v>
       </c>
       <c r="H29" t="n">
-        <v>22.60595823830538</v>
+        <v>22.67011743958247</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -1633,16 +1633,16 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1.549682382437454</v>
+        <v>1.562871425262642</v>
       </c>
       <c r="F30" t="n">
-        <v>1201.028300603457</v>
+        <v>1210.662974764501</v>
       </c>
       <c r="G30" t="n">
-        <v>0.5710797012942002</v>
+        <v>0.5721959215080588</v>
       </c>
       <c r="H30" t="n">
-        <v>17.11192700119544</v>
+        <v>17.16049329343311</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -1674,16 +1674,16 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.350015958929949</v>
+        <v>1.361505679934788</v>
       </c>
       <c r="F31" t="n">
-        <v>1046.283671644529</v>
+        <v>1054.676981117854</v>
       </c>
       <c r="G31" t="n">
-        <v>0.4974998228991074</v>
+        <v>0.4984722254490351</v>
       </c>
       <c r="H31" t="n">
-        <v>14.90716730589557</v>
+        <v>14.94947614941127</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -1715,16 +1715,16 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.264350732014215</v>
+        <v>1.275111373080024</v>
       </c>
       <c r="F32" t="n">
-        <v>979.8917689719682</v>
+        <v>987.752481217145</v>
       </c>
       <c r="G32" t="n">
-        <v>0.4659309848048661</v>
+        <v>0.4668416835768274</v>
       </c>
       <c r="H32" t="n">
-        <v>13.96123339910138</v>
+        <v>14.00085753607906</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -1756,16 +1756,16 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>6.732865430476495</v>
+        <v>6.790167527363336</v>
       </c>
       <c r="F33" t="n">
-        <v>5218.076954373192</v>
+        <v>5259.936476675377</v>
       </c>
       <c r="G33" t="n">
-        <v>2.481155379956814</v>
+        <v>2.486004993376072</v>
       </c>
       <c r="H33" t="n">
-        <v>74.34575181356722</v>
+        <v>74.55675654121146</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -1793,16 +1793,16 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>4.737271141018293</v>
+        <v>4.777589126623973</v>
       </c>
       <c r="F34" t="n">
-        <v>3671.459889108671</v>
+        <v>3700.912417187197</v>
       </c>
       <c r="G34" t="n">
-        <v>1.745750883349016</v>
+        <v>1.749163090822648</v>
       </c>
       <c r="H34" t="n">
-        <v>52.30996936260839</v>
+        <v>52.4584331364298</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -1834,16 +1834,16 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>9.257583787354559</v>
+        <v>9.336373267060479</v>
       </c>
       <c r="F35" t="n">
-        <v>7174.77352135602</v>
+        <v>7232.329704498128</v>
       </c>
       <c r="G35" t="n">
-        <v>3.411549518277087</v>
+        <v>3.418217660252973</v>
       </c>
       <c r="H35" t="n">
-        <v>102.224236272958</v>
+        <v>102.5143644462063</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -1871,16 +1871,16 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>7.033242315102685</v>
+        <v>7.093100860843564</v>
       </c>
       <c r="F36" t="n">
-        <v>5450.87377989943</v>
+        <v>5494.600803280554</v>
       </c>
       <c r="G36" t="n">
-        <v>2.591848476165428</v>
+        <v>2.596914447954968</v>
       </c>
       <c r="H36" t="n">
-        <v>77.66257813098613</v>
+        <v>77.88299652433969</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -1912,16 +1912,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2.831983488017804</v>
+        <v>2.856085943882715</v>
       </c>
       <c r="F37" t="n">
-        <v>2194.831892416138</v>
+        <v>2212.43887965837</v>
       </c>
       <c r="G37" t="n">
-        <v>1.043625651047376</v>
+        <v>1.045665499498124</v>
       </c>
       <c r="H37" t="n">
-        <v>31.27137230673033</v>
+        <v>31.36012529162571</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -1953,16 +1953,16 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>5.989426425276149</v>
+        <v>6.04040125881186</v>
       </c>
       <c r="F38" t="n">
-        <v>4641.899993659365</v>
+        <v>4679.13741248122</v>
       </c>
       <c r="G38" t="n">
-        <v>2.207187674771785</v>
+        <v>2.211501796760329</v>
       </c>
       <c r="H38" t="n">
-        <v>66.13653800399427</v>
+        <v>66.32424371523301</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -1990,16 +1990,16 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.2731525586047452</v>
+        <v>0.2754773064621315</v>
       </c>
       <c r="F39" t="n">
-        <v>211.6975433043677</v>
+        <v>213.3957854292133</v>
       </c>
       <c r="G39" t="n">
-        <v>0.1006605503991117</v>
+        <v>0.1008572993658515</v>
       </c>
       <c r="H39" t="n">
-        <v>3.016209447559885</v>
+        <v>3.024769915916462</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
@@ -2031,16 +2031,16 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>15.16777052301413</v>
+        <v>15.29686044270491</v>
       </c>
       <c r="F40" t="n">
-        <v>11755.26150519533</v>
+        <v>11849.56245866357</v>
       </c>
       <c r="G40" t="n">
-        <v>5.589536255922397</v>
+        <v>5.600461444354243</v>
       </c>
       <c r="H40" t="n">
-        <v>167.4857925466809</v>
+        <v>167.9611430976242</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -2070,16 +2070,16 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0.05730911330205199</v>
+        <v>0.057796859976945</v>
       </c>
       <c r="F41" t="n">
-        <v>44.41546712962228</v>
+        <v>44.77176897365867</v>
       </c>
       <c r="G41" t="n">
-        <v>0.02111921218396826</v>
+        <v>0.02116049134777637</v>
       </c>
       <c r="H41" t="n">
-        <v>0.6328195815279345</v>
+        <v>0.6346156213821151</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -2109,16 +2109,16 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.01533107714259406</v>
+        <v>0.01546155683228587</v>
       </c>
       <c r="F42" t="n">
-        <v>11.8818267626378</v>
+        <v>11.97714295224769</v>
       </c>
       <c r="G42" t="n">
-        <v>0.005649717357161125</v>
+        <v>0.005660760170870715</v>
       </c>
       <c r="H42" t="n">
-        <v>0.1692890677630451</v>
+        <v>0.1697695360418795</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -2150,16 +2150,16 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>1.561530729542375</v>
+        <v>1.574820611289154</v>
       </c>
       <c r="F43" t="n">
-        <v>1210.210956596835</v>
+        <v>1219.919294189675</v>
       </c>
       <c r="G43" t="n">
-        <v>0.5754459835622354</v>
+        <v>0.5765707380171122</v>
       </c>
       <c r="H43" t="n">
-        <v>17.24275900765102</v>
+        <v>17.29169662124358</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -2189,16 +2189,16 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.2905804149191108</v>
+        <v>0.2930534877518712</v>
       </c>
       <c r="F44" t="n">
-        <v>225.2044070079226</v>
+        <v>227.0110014095327</v>
       </c>
       <c r="G44" t="n">
-        <v>0.107082960270774</v>
+        <v>0.1072922623398644</v>
       </c>
       <c r="H44" t="n">
-        <v>3.208651602258952</v>
+        <v>3.217758250954638</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -2228,16 +2228,16 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1.512942197502034</v>
+        <v>1.52581855192737</v>
       </c>
       <c r="F45" t="n">
-        <v>1172.554077458833</v>
+        <v>1181.960330884635</v>
       </c>
       <c r="G45" t="n">
-        <v>0.5575404273037552</v>
+        <v>0.5586301839448949</v>
       </c>
       <c r="H45" t="n">
-        <v>16.70623394845409</v>
+        <v>16.75364882140252</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -2269,16 +2269,16 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>8.530109809059848</v>
+        <v>8.602707900334009</v>
       </c>
       <c r="F46" t="n">
-        <v>6610.969708571142</v>
+        <v>6664.003045671587</v>
       </c>
       <c r="G46" t="n">
-        <v>3.143465150444898</v>
+        <v>3.149609300425903</v>
       </c>
       <c r="H46" t="n">
-        <v>94.19131175701681</v>
+        <v>94.45864124939082</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -2308,16 +2308,16 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>2.374376069194457</v>
+        <v>2.394583918235257</v>
       </c>
       <c r="F47" t="n">
-        <v>1840.178921631599</v>
+        <v>1854.940875443207</v>
       </c>
       <c r="G47" t="n">
-        <v>0.874990896049447</v>
+        <v>0.8767011346076048</v>
       </c>
       <c r="H47" t="n">
-        <v>26.21837250721652</v>
+        <v>26.29278429851911</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
@@ -2349,16 +2349,16 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>3.196469218253392</v>
+        <v>3.223673740802158</v>
       </c>
       <c r="F48" t="n">
-        <v>2477.314084927521</v>
+        <v>2497.187150315601</v>
       </c>
       <c r="G48" t="n">
-        <v>1.177943756306886</v>
+        <v>1.180246140067751</v>
       </c>
       <c r="H48" t="n">
-        <v>35.2961023186756</v>
+        <v>35.39627810936505</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -2386,16 +2386,16 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>1.081759807442837</v>
+        <v>1.09096645294668</v>
       </c>
       <c r="F49" t="n">
-        <v>838.3809211244844</v>
+        <v>845.1064303769876</v>
       </c>
       <c r="G49" t="n">
-        <v>0.3986436672372489</v>
+        <v>0.399422847651791</v>
       </c>
       <c r="H49" t="n">
-        <v>11.94502504181953</v>
+        <v>11.97892686798708</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
@@ -2423,16 +2423,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>5.921392470789153</v>
+        <v>5.971788280608976</v>
       </c>
       <c r="F50" t="n">
-        <v>4589.172605382382</v>
+        <v>4625.987043939519</v>
       </c>
       <c r="G50" t="n">
-        <v>2.182116208199667</v>
+        <v>2.186381326031487</v>
       </c>
       <c r="H50" t="n">
-        <v>65.38529241541019</v>
+        <v>65.57086597544107</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -2460,16 +2460,16 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>2.369910050488812</v>
+        <v>2.390079890072105</v>
       </c>
       <c r="F51" t="n">
-        <v>1836.717686684378</v>
+        <v>1851.451874361832</v>
       </c>
       <c r="G51" t="n">
-        <v>0.8733451056479573</v>
+        <v>0.8750521273776309</v>
       </c>
       <c r="H51" t="n">
-        <v>26.1690577697115</v>
+        <v>26.24332959805329</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -2501,16 +2501,16 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>2.952406632727396</v>
+        <v>2.977533986409328</v>
       </c>
       <c r="F52" t="n">
-        <v>2288.161729835708</v>
+        <v>2306.517411023383</v>
       </c>
       <c r="G52" t="n">
-        <v>1.0880032693517</v>
+        <v>1.090129857351166</v>
       </c>
       <c r="H52" t="n">
-        <v>32.60111063145099</v>
+        <v>32.69363761924976</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
@@ -2542,16 +2542,16 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>2.320121492559983</v>
+        <v>2.339867591565074</v>
       </c>
       <c r="F53" t="n">
-        <v>1798.130768582076</v>
+        <v>1812.555411248375</v>
       </c>
       <c r="G53" t="n">
-        <v>0.8549973232409041</v>
+        <v>0.856668482788595</v>
       </c>
       <c r="H53" t="n">
-        <v>25.61928177184047</v>
+        <v>25.6919932511519</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
@@ -2579,16 +2579,16 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>2.428324549870182</v>
+        <v>2.448991543738958</v>
       </c>
       <c r="F54" t="n">
-        <v>1881.98984552535</v>
+        <v>1897.087207363295</v>
       </c>
       <c r="G54" t="n">
-        <v>0.8948716684734496</v>
+        <v>0.8966207655619548</v>
       </c>
       <c r="H54" t="n">
-        <v>26.8140832720444</v>
+        <v>26.89018578225184</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
@@ -2620,16 +2620,16 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>2.307339006297756</v>
+        <v>2.326976315886634</v>
       </c>
       <c r="F55" t="n">
-        <v>1788.224140110579</v>
+        <v>1802.569311463471</v>
       </c>
       <c r="G55" t="n">
-        <v>0.8502867982859463</v>
+        <v>0.8519487507357387</v>
       </c>
       <c r="H55" t="n">
-        <v>25.47813481752616</v>
+        <v>25.55044569953118</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
@@ -2661,16 +2661,16 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>2.501356319884388</v>
+        <v>2.522644872858434</v>
       </c>
       <c r="F56" t="n">
-        <v>1938.590619721352</v>
+        <v>1954.142034179071</v>
       </c>
       <c r="G56" t="n">
-        <v>0.9217849003132343</v>
+        <v>0.9235866014323025</v>
       </c>
       <c r="H56" t="n">
-        <v>27.62051582045254</v>
+        <v>27.69890711089125</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>2.831403014450368</v>
+        <v>2.855500530244345</v>
       </c>
       <c r="F57" t="n">
-        <v>2194.382016128629</v>
+        <v>2211.985394617674</v>
       </c>
       <c r="G57" t="n">
-        <v>1.043411737673878</v>
+        <v>1.045451168021779</v>
       </c>
       <c r="H57" t="n">
-        <v>31.26496257379001</v>
+        <v>31.35369736742455</v>
       </c>
       <c r="I57" t="n">
         <v>0</v>
@@ -2739,16 +2739,16 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>4.70417259857583</v>
+        <v>4.74420888872961</v>
       </c>
       <c r="F58" t="n">
-        <v>3645.807996540145</v>
+        <v>3675.05474441927</v>
       </c>
       <c r="G58" t="n">
-        <v>1.733553606850437</v>
+        <v>1.736941973778909</v>
       </c>
       <c r="H58" t="n">
-        <v>51.94448814096603</v>
+        <v>52.09191462201451</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
@@ -2776,16 +2776,16 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>12.17875730952931</v>
+        <v>12.2824083240949</v>
       </c>
       <c r="F59" t="n">
-        <v>9438.729097622378</v>
+        <v>9514.446779722339</v>
       </c>
       <c r="G59" t="n">
-        <v>4.488042947984342</v>
+        <v>4.496815181074315</v>
       </c>
       <c r="H59" t="n">
-        <v>134.480464158738</v>
+        <v>134.8621404894131</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
@@ -2817,16 +2817,16 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>11.90755020505613</v>
+        <v>12.0088930292245</v>
       </c>
       <c r="F60" t="n">
-        <v>9228.539311928744</v>
+        <v>9302.570847226185</v>
       </c>
       <c r="G60" t="n">
-        <v>4.388099324469024</v>
+        <v>4.396676209885039</v>
       </c>
       <c r="H60" t="n">
-        <v>131.4857368284248</v>
+        <v>131.8589136605099</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
@@ -2858,16 +2858,16 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>0.3496010061132409</v>
+        <v>0.3525763916524107</v>
       </c>
       <c r="F61" t="n">
-        <v>270.9462965218479</v>
+        <v>273.119833340266</v>
       </c>
       <c r="G61" t="n">
-        <v>0.1288328761388917</v>
+        <v>0.1290846901310509</v>
       </c>
       <c r="H61" t="n">
-        <v>3.860369693439044</v>
+        <v>3.871326018827018</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
@@ -2899,16 +2899,16 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>6.991142413205311</v>
+        <v>7.050642655075287</v>
       </c>
       <c r="F62" t="n">
-        <v>5418.245691517767</v>
+        <v>5461.710971790717</v>
       </c>
       <c r="G62" t="n">
-        <v>2.576334071181216</v>
+        <v>2.581369718850068</v>
       </c>
       <c r="H62" t="n">
-        <v>77.19770192553482</v>
+        <v>77.41680092873973</v>
       </c>
       <c r="I62" t="n">
         <v>0</v>
@@ -2940,16 +2940,16 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>7.021842485230557</v>
+        <v>7.0816040091611</v>
       </c>
       <c r="F63" t="n">
-        <v>5442.038731904558</v>
+        <v>5485.694880277509</v>
       </c>
       <c r="G63" t="n">
-        <v>2.587647479208027</v>
+        <v>2.592705239815242</v>
       </c>
       <c r="H63" t="n">
-        <v>77.53669875934008</v>
+        <v>77.75675988736158</v>
       </c>
       <c r="I63" t="n">
         <v>0</v>
@@ -2977,16 +2977,16 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1.527106024576844</v>
+        <v>1.540102924531547</v>
       </c>
       <c r="F64" t="n">
-        <v>1183.531266961553</v>
+        <v>1193.025579613135</v>
       </c>
       <c r="G64" t="n">
-        <v>0.5627599963910094</v>
+        <v>0.5638599550898035</v>
       </c>
       <c r="H64" t="n">
-        <v>16.86263398300756</v>
+        <v>16.91049274335333</v>
       </c>
       <c r="I64" t="n">
         <v>0</v>
@@ -3018,16 +3018,16 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>12.99802032451594</v>
+        <v>13.10864392593082</v>
       </c>
       <c r="F65" t="n">
-        <v>10073.67086232368</v>
+        <v>10154.48206055231</v>
       </c>
       <c r="G65" t="n">
-        <v>4.78995286394417</v>
+        <v>4.799315203722104</v>
       </c>
       <c r="H65" t="n">
-        <v>143.5269430148136</v>
+        <v>143.9342946499768</v>
       </c>
       <c r="I65" t="n">
         <v>0</v>
@@ -3055,16 +3055,16 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>3.68484697301795</v>
+        <v>3.716207982639984</v>
       </c>
       <c r="F66" t="n">
-        <v>2855.81455164948</v>
+        <v>2878.723955546845</v>
       </c>
       <c r="G66" t="n">
-        <v>1.357917811977251</v>
+        <v>1.360571969184611</v>
       </c>
       <c r="H66" t="n">
-        <v>40.68887480592358</v>
+        <v>40.80435611747047</v>
       </c>
       <c r="I66" t="n">
         <v>0</v>
@@ -3096,16 +3096,16 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>7.266910215056429</v>
+        <v>7.32875746248172</v>
       </c>
       <c r="F67" t="n">
-        <v>5631.970089669159</v>
+        <v>5677.149871448669</v>
       </c>
       <c r="G67" t="n">
-        <v>2.677958375807194</v>
+        <v>2.68319265617203</v>
       </c>
       <c r="H67" t="n">
-        <v>80.24278946318529</v>
+        <v>80.47053089492357</v>
       </c>
       <c r="I67" t="n">
         <v>0</v>
@@ -3137,16 +3137,16 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>11.64656000433002</v>
+        <v>11.74568159208496</v>
       </c>
       <c r="F68" t="n">
-        <v>9026.267787903409</v>
+        <v>9098.676696800927</v>
       </c>
       <c r="G68" t="n">
-        <v>4.291920773592024</v>
+        <v>4.3003096704621</v>
       </c>
       <c r="H68" t="n">
-        <v>128.6038267588295</v>
+        <v>128.9688242849423</v>
       </c>
       <c r="I68" t="n">
         <v>0</v>
@@ -3178,16 +3178,16 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>9.027369361780732</v>
+        <v>9.104199531733517</v>
       </c>
       <c r="F69" t="n">
-        <v>6996.353708683017</v>
+        <v>7052.478604406419</v>
       </c>
       <c r="G69" t="n">
-        <v>3.326712272118644</v>
+        <v>3.333214593023606</v>
       </c>
       <c r="H69" t="n">
-        <v>99.68215894219999</v>
+        <v>99.9650723074658</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
@@ -3219,16 +3219,16 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>7.215885255827838</v>
+        <v>7.277298239788485</v>
       </c>
       <c r="F70" t="n">
-        <v>5592.424941107637</v>
+        <v>5637.28749084596</v>
       </c>
       <c r="G70" t="n">
-        <v>2.659154962547728</v>
+        <v>2.664352490160233</v>
       </c>
       <c r="H70" t="n">
-        <v>79.67936086528044</v>
+        <v>79.9055031995135</v>
       </c>
       <c r="I70" t="n">
         <v>0</v>
@@ -3260,16 +3260,16 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>5.345088773755815</v>
+        <v>5.390579775831693</v>
       </c>
       <c r="F71" t="n">
-        <v>4142.528146028078</v>
+        <v>4175.759593380993</v>
       </c>
       <c r="G71" t="n">
-        <v>1.969740209829953</v>
+        <v>1.973590222061099</v>
       </c>
       <c r="H71" t="n">
-        <v>59.02162273372133</v>
+        <v>59.18913521613653</v>
       </c>
       <c r="I71" t="n">
         <v>0</v>
@@ -3301,16 +3301,16 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.7664194573546333</v>
+        <v>0.7729423029457242</v>
       </c>
       <c r="F72" t="n">
-        <v>593.9871737089774</v>
+        <v>598.7521511768089</v>
       </c>
       <c r="G72" t="n">
-        <v>0.2824363238609282</v>
+        <v>0.2829883678772669</v>
       </c>
       <c r="H72" t="n">
-        <v>8.462968907376254</v>
+        <v>8.486988120238742</v>
       </c>
       <c r="I72" t="n">
         <v>0</v>
@@ -3342,16 +3342,16 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>5.543700609148021</v>
+        <v>5.590881957684426</v>
       </c>
       <c r="F73" t="n">
-        <v>4296.455452539709</v>
+        <v>4330.921708026362</v>
       </c>
       <c r="G73" t="n">
-        <v>2.042931457603276</v>
+        <v>2.046924527890336</v>
       </c>
       <c r="H73" t="n">
-        <v>61.2147374369578</v>
+        <v>61.38847431788872</v>
       </c>
       <c r="I73" t="n">
         <v>0</v>
@@ -3383,16 +3383,16 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>6.223343542828761</v>
+        <v>6.276309199065379</v>
       </c>
       <c r="F74" t="n">
-        <v>4823.189451013704</v>
+        <v>4861.881177649324</v>
       </c>
       <c r="G74" t="n">
-        <v>2.293389414677077</v>
+        <v>2.297872024749069</v>
       </c>
       <c r="H74" t="n">
-        <v>68.71950125277088</v>
+        <v>68.91453781269612</v>
       </c>
       <c r="I74" t="n">
         <v>0</v>
@@ -3424,16 +3424,16 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>12.77684744651185</v>
+        <v>12.88558868884816</v>
       </c>
       <c r="F75" t="n">
-        <v>9902.25839177586</v>
+        <v>9981.694515512298</v>
       </c>
       <c r="G75" t="n">
-        <v>4.708447555446879</v>
+        <v>4.717650586682676</v>
       </c>
       <c r="H75" t="n">
-        <v>141.0847044153208</v>
+        <v>141.4851245998441</v>
       </c>
       <c r="I75" t="n">
         <v>0</v>
@@ -3461,16 +3461,16 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>6.100136758269887</v>
+        <v>6.152053825685003</v>
       </c>
       <c r="F76" t="n">
-        <v>4727.702248780533</v>
+        <v>4765.627975051076</v>
       </c>
       <c r="G76" t="n">
-        <v>2.247985986004896</v>
+        <v>2.252379851501368</v>
       </c>
       <c r="H76" t="n">
-        <v>67.35902537595226</v>
+        <v>67.55020069507337</v>
       </c>
       <c r="I76" t="n">
         <v>0</v>
@@ -3498,16 +3498,16 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>4.83582345036739</v>
+        <v>4.876980195176253</v>
       </c>
       <c r="F77" t="n">
-        <v>3747.839484110545</v>
+        <v>3777.904730772952</v>
       </c>
       <c r="G77" t="n">
-        <v>1.782068792668716</v>
+        <v>1.785551986348047</v>
       </c>
       <c r="H77" t="n">
-        <v>53.39820522606898</v>
+        <v>53.5497575809561</v>
       </c>
       <c r="I77" t="n">
         <v>0</v>
@@ -3539,16 +3539,16 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>11.30417484138024</v>
+        <v>11.40038245608853</v>
       </c>
       <c r="F78" t="n">
-        <v>8760.913883766971</v>
+        <v>8831.194118037998</v>
       </c>
       <c r="G78" t="n">
-        <v>4.165747037328494</v>
+        <v>4.173889317700005</v>
       </c>
       <c r="H78" t="n">
-        <v>124.8231359724668</v>
+        <v>125.1774033139126</v>
       </c>
       <c r="I78" t="n">
         <v>0</v>
@@ -3576,16 +3576,16 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>9.49997973088831</v>
+        <v>9.580832194999221</v>
       </c>
       <c r="F79" t="n">
-        <v>7362.634202603347</v>
+        <v>7421.697408112179</v>
       </c>
       <c r="G79" t="n">
-        <v>3.500875824269626</v>
+        <v>3.507718561541933</v>
       </c>
       <c r="H79" t="n">
-        <v>104.9008245398456</v>
+        <v>105.1985492842378</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
@@ -3617,16 +3617,16 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>1.737222999034274</v>
+        <v>1.752008163102963</v>
       </c>
       <c r="F80" t="n">
-        <v>1346.37523796572</v>
+        <v>1357.175888181709</v>
       </c>
       <c r="G80" t="n">
-        <v>0.6401910503841175</v>
+        <v>0.6414423541625357</v>
       </c>
       <c r="H80" t="n">
-        <v>19.18279093963257</v>
+        <v>19.23723466323155</v>
       </c>
       <c r="I80" t="n">
         <v>0</v>
@@ -3658,16 +3658,16 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>2.654256344782261</v>
+        <v>2.676846199893275</v>
       </c>
       <c r="F81" t="n">
-        <v>2057.090551795638</v>
+        <v>2073.592575197422</v>
       </c>
       <c r="G81" t="n">
-        <v>0.9781307047657285</v>
+        <v>0.9800425381938215</v>
       </c>
       <c r="H81" t="n">
-        <v>29.30887086182819</v>
+        <v>29.39205396471803</v>
       </c>
       <c r="I81" t="n">
         <v>0</v>
@@ -3699,16 +3699,16 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>2.665201976653578</v>
+        <v>2.687884987987194</v>
       </c>
       <c r="F82" t="n">
-        <v>2065.573589171387</v>
+        <v>2082.143663746513</v>
       </c>
       <c r="G82" t="n">
-        <v>0.9821643233794939</v>
+        <v>0.9840840408358479</v>
       </c>
       <c r="H82" t="n">
-        <v>29.42973488102172</v>
+        <v>29.51326101490441</v>
       </c>
       <c r="I82" t="n">
         <v>0</v>
@@ -3740,16 +3740,16 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>6.933081572810671</v>
+        <v>6.992087670179351</v>
       </c>
       <c r="F83" t="n">
-        <v>5373.247624041293</v>
+        <v>5416.351928820216</v>
       </c>
       <c r="G83" t="n">
-        <v>2.554937837094489</v>
+        <v>2.55993166413759</v>
       </c>
       <c r="H83" t="n">
-        <v>76.55658161339537</v>
+        <v>76.77386101793036</v>
       </c>
       <c r="I83" t="n">
         <v>0</v>
@@ -3781,16 +3781,16 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>8.833799832732321</v>
+        <v>8.908982570365453</v>
       </c>
       <c r="F84" t="n">
-        <v>6846.33426912593</v>
+        <v>6901.255705749982</v>
       </c>
       <c r="G84" t="n">
-        <v>3.255379184788066</v>
+        <v>3.261742079559972</v>
       </c>
       <c r="H84" t="n">
-        <v>97.54472246780855</v>
+        <v>97.8215694581209</v>
       </c>
       <c r="I84" t="n">
         <v>0</v>
@@ -3818,16 +3818,16 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>9.097909401995063</v>
+        <v>9.175339924224746</v>
       </c>
       <c r="F85" t="n">
-        <v>7051.023353066543</v>
+        <v>7107.586809697395</v>
       </c>
       <c r="G85" t="n">
-        <v>3.352707267218463</v>
+        <v>3.359260397381064</v>
       </c>
       <c r="H85" t="n">
-        <v>100.461077289818</v>
+        <v>100.7462013452628</v>
       </c>
       <c r="I85" t="n">
         <v>0</v>
@@ -3859,16 +3859,16 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>6.457274874734304</v>
+        <v>6.512231474676114</v>
       </c>
       <c r="F86" t="n">
-        <v>5004.489924701521</v>
+        <v>5044.636047545002</v>
       </c>
       <c r="G86" t="n">
-        <v>2.379596392679362</v>
+        <v>2.38424750107405</v>
       </c>
       <c r="H86" t="n">
-        <v>71.30262145712508</v>
+        <v>71.50498931127115</v>
       </c>
       <c r="I86" t="n">
         <v>0</v>
@@ -3896,16 +3896,16 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>8.543289939455034</v>
+        <v>8.616000204220564</v>
       </c>
       <c r="F87" t="n">
-        <v>6621.184517618523</v>
+        <v>6674.299798121137</v>
       </c>
       <c r="G87" t="n">
-        <v>3.148322213466919</v>
+        <v>3.154475856959339</v>
       </c>
       <c r="H87" t="n">
-        <v>94.33684959978318</v>
+        <v>94.60459215100441</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
@@ -3937,16 +3937,16 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>7.115275469776815</v>
+        <v>7.17583218362833</v>
       </c>
       <c r="F88" t="n">
-        <v>5514.450769257071</v>
+        <v>5558.687808591772</v>
       </c>
       <c r="G88" t="n">
-        <v>2.622078844594359</v>
+        <v>2.627203904018469</v>
       </c>
       <c r="H88" t="n">
-        <v>78.56840591080309</v>
+        <v>78.7913951833746</v>
       </c>
       <c r="I88" t="n">
         <v>0</v>
@@ -3978,16 +3978,16 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.3951708646267455</v>
+        <v>0.3985340863054654</v>
       </c>
       <c r="F89" t="n">
-        <v>306.263655963275</v>
+        <v>308.7205093862913</v>
       </c>
       <c r="G89" t="n">
-        <v>0.1456260083496203</v>
+        <v>0.1459106458404984</v>
       </c>
       <c r="H89" t="n">
-        <v>4.363561895756919</v>
+        <v>4.375946358374167</v>
       </c>
       <c r="I89" t="n">
         <v>0</v>
@@ -4019,16 +4019,16 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>6.202305532404567</v>
+        <v>6.255092138264833</v>
       </c>
       <c r="F90" t="n">
-        <v>4806.884660949934</v>
+        <v>4845.445590221567</v>
       </c>
       <c r="G90" t="n">
-        <v>2.285636612640874</v>
+        <v>2.290104069251372</v>
       </c>
       <c r="H90" t="n">
-        <v>68.48719500520842</v>
+        <v>68.68157224412747</v>
       </c>
       <c r="I90" t="n">
         <v>0</v>
@@ -4060,16 +4060,16 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>10.55808059236474</v>
+        <v>10.64793834523963</v>
       </c>
       <c r="F91" t="n">
-        <v>8182.679067307634</v>
+        <v>8248.320689774728</v>
       </c>
       <c r="G91" t="n">
-        <v>3.890800838252573</v>
+        <v>3.898405714642486</v>
       </c>
       <c r="H91" t="n">
-        <v>116.5846024065932</v>
+        <v>116.9154875170914</v>
       </c>
       <c r="I91" t="n">
         <v>0</v>
@@ -4084,7 +4084,7 @@
         <v>44100.52733557689</v>
       </c>
       <c r="B92" s="2" t="n">
-        <v>44100.53912830922</v>
+        <v>44100.5363005928</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -4093,20 +4093,20 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>POINT (4.01626496035667 51.5211460393743)</t>
+          <t>POINT (4.01810085879421 51.5271727057482)</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>10.69613021280485</v>
+        <v>8.200566592802396</v>
       </c>
       <c r="F92" t="n">
-        <v>8289.66970157072</v>
+        <v>6352.488237819693</v>
       </c>
       <c r="G92" t="n">
-        <v>3.941674060203622</v>
+        <v>3.002377984484893</v>
       </c>
       <c r="H92" t="n">
-        <v>118.1089760775198</v>
+        <v>90.04308721623059</v>
       </c>
       <c r="I92" t="n">
         <v>0</v>
@@ -4118,32 +4118,32 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>44100.53912830922</v>
+        <v>44100.5363005928</v>
       </c>
       <c r="B93" s="2" t="n">
-        <v>44100.54149369823</v>
+        <v>44100.5524464753</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>POINT (4.0162304852485 51.5211475486708)</t>
+          <t>POINT (4.01810085879421 51.5271727057482)</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>POINT (4.01567956925141 51.519343094515)</t>
+          <t>POINT (4.03803692928046 51.5255707663223)</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>2.145432296522062</v>
+        <v>14.76911877022747</v>
       </c>
       <c r="F93" t="n">
-        <v>1662.743885070348</v>
+        <v>11440.7525637318</v>
       </c>
       <c r="G93" t="n">
-        <v>0.7906219037092954</v>
+        <v>5.407245529080723</v>
       </c>
       <c r="H93" t="n">
-        <v>23.69032601002827</v>
+        <v>162.166483797935</v>
       </c>
       <c r="I93" t="n">
         <v>0</v>
@@ -4159,32 +4159,32 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>44100.54149369823</v>
+        <v>44100.5524464753</v>
       </c>
       <c r="B94" s="2" t="n">
-        <v>44100.55031167286</v>
+        <v>44100.55608690767</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>POINT (4.01567956925141 51.519343094515)</t>
+          <t>POINT (4.03803692928046 51.5255707663223)</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>POINT (4.01333072505197 51.5126539509607)</t>
+          <t>POINT (4.04252985126733 51.5252000579642)</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>7.997994209795595</v>
+        <v>3.330011717035138</v>
       </c>
       <c r="F94" t="n">
-        <v>6198.571722174107</v>
+        <v>2579.560817542324</v>
       </c>
       <c r="G94" t="n">
-        <v>2.947373085408372</v>
+        <v>1.219178425692702</v>
       </c>
       <c r="H94" t="n">
-        <v>88.31557656057211</v>
+        <v>36.56388032501345</v>
       </c>
       <c r="I94" t="n">
         <v>0</v>
@@ -4200,32 +4200,32 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>44100.55031167286</v>
+        <v>44100.55608690767</v>
       </c>
       <c r="B95" s="2" t="n">
-        <v>44100.55214175794</v>
+        <v>44100.5645038951</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>POINT (4.01333072505197 51.5126539509607)</t>
+          <t>POINT (4.04252985126733 51.5252000579642)</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>POINT (4.01265125183207 51.5112974704514)</t>
+          <t>POINT (4.05295425491929 51.5245374927562)</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>1.659906099393021</v>
+        <v>7.699268666637875</v>
       </c>
       <c r="F95" t="n">
-        <v>1286.453420650991</v>
+        <v>5964.162730817403</v>
       </c>
       <c r="G95" t="n">
-        <v>0.6116986879116819</v>
+        <v>2.818843610150843</v>
       </c>
       <c r="H95" t="n">
-        <v>18.32904105969589</v>
+        <v>84.53878304189257</v>
       </c>
       <c r="I95" t="n">
         <v>0</v>
@@ -4233,40 +4233,36 @@
       <c r="J95" t="n">
         <v>10</v>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
+      <c r="K95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>44100.55214175794</v>
+        <v>44100.5645038951</v>
       </c>
       <c r="B96" s="2" t="n">
-        <v>44100.55614866562</v>
+        <v>44100.57390259874</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>POINT (4.01265125183207 51.5112974704514)</t>
+          <t>POINT (4.05295425491929 51.5245374927562)</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>POINT (4.01057561055691 51.508468187284)</t>
+          <t>POINT (4.06456672200451 51.5236447375633)</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>3.634306711747289</v>
+        <v>8.597273655679288</v>
       </c>
       <c r="F96" t="n">
-        <v>2816.645051485938</v>
+        <v>6659.793461436336</v>
       </c>
       <c r="G96" t="n">
-        <v>1.339293015644391</v>
+        <v>3.147619723224478</v>
       </c>
       <c r="H96" t="n">
-        <v>40.13079831959553</v>
+        <v>94.39897265712328</v>
       </c>
       <c r="I96" t="n">
         <v>0</v>
@@ -4274,36 +4270,40 @@
       <c r="J96" t="n">
         <v>10</v>
       </c>
-      <c r="K96" t="inlineStr"/>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>44100.55614866562</v>
+        <v>44100.57390259874</v>
       </c>
       <c r="B97" s="2" t="n">
-        <v>44100.5612915991</v>
+        <v>44100.60192844577</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>POINT (4.01057561055691 51.508468187284)</t>
+          <t>POINT (4.06456672200451 51.5236447375633)</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>POINT (4.00717730543896 51.5050838720503)</t>
+          <t>POINT (4.09901897625955 51.5202181713621)</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>4.664693871278195</v>
+        <v>25.6360755349437</v>
       </c>
       <c r="F97" t="n">
-        <v>3615.211359893833</v>
+        <v>19858.73371754295</v>
       </c>
       <c r="G97" t="n">
-        <v>1.719005141853686</v>
+        <v>9.385837907996811</v>
       </c>
       <c r="H97" t="n">
-        <v>51.50855552020512</v>
+        <v>281.4868166885854</v>
       </c>
       <c r="I97" t="n">
         <v>0</v>
@@ -4311,40 +4311,36 @@
       <c r="J97" t="n">
         <v>10</v>
       </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
+      <c r="K97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>44100.5612915991</v>
+        <v>44100.60192844577</v>
       </c>
       <c r="B98" s="2" t="n">
-        <v>44100.56228592581</v>
+        <v>44100.60995531583</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>POINT (4.00717730543896 51.5050838720503)</t>
+          <t>POINT (4.09901897625955 51.5202181713621)</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>POINT (4.00668012620939 51.50437678529)</t>
+          <t>POINT (4.10896407090242 51.5196172513597)</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.9018646148175521</v>
+        <v>7.342416706867411</v>
       </c>
       <c r="F98" t="n">
-        <v>698.9593080468652</v>
+        <v>5687.730870724785</v>
       </c>
       <c r="G98" t="n">
-        <v>0.3323497645404221</v>
+        <v>2.68819355622303</v>
       </c>
       <c r="H98" t="n">
-        <v>9.958583533394989</v>
+        <v>80.62051083844645</v>
       </c>
       <c r="I98" t="n">
         <v>0</v>
@@ -4360,32 +4356,32 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>44100.56228592581</v>
+        <v>44100.60995531583</v>
       </c>
       <c r="B99" s="2" t="n">
-        <v>44100.56487037678</v>
+        <v>44100.62185406171</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>POINT (4.00668012620939 51.50437678529)</t>
+          <t>POINT (4.10896407090242 51.5196172513597)</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>POINT (4.00539622618623 51.5025366544588)</t>
+          <t>POINT (4.12374892768784 51.5190679384549)</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>2.344123766586404</v>
+        <v>10.88413662776244</v>
       </c>
       <c r="F99" t="n">
-        <v>1816.7329097835</v>
+        <v>8431.289365713174</v>
       </c>
       <c r="G99" t="n">
-        <v>0.8638424984484077</v>
+        <v>3.984882242187901</v>
       </c>
       <c r="H99" t="n">
-        <v>25.88432006871581</v>
+        <v>119.5089696012972</v>
       </c>
       <c r="I99" t="n">
         <v>0</v>
@@ -4401,32 +4397,32 @@
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>44100.56487037678</v>
+        <v>44100.62185406171</v>
       </c>
       <c r="B100" s="2" t="n">
-        <v>44100.56663462016</v>
+        <v>44100.62823132874</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>POINT (4.00539622618623 51.5025366544588)</t>
+          <t>POINT (4.12374892768784 51.5190679384549)</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>POINT (4.00482311611334 51.5012141033689)</t>
+          <t>POINT (4.13166341354231 51.5194499362428)</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>1.600186996182947</v>
+        <v>5.833475756524325</v>
       </c>
       <c r="F100" t="n">
-        <v>1240.17017323917</v>
+        <v>4518.844607800258</v>
       </c>
       <c r="G100" t="n">
-        <v>0.5896913601636882</v>
+        <v>2.135742571607893</v>
       </c>
       <c r="H100" t="n">
-        <v>17.66960983782268</v>
+        <v>64.05217985269158</v>
       </c>
       <c r="I100" t="n">
         <v>0</v>
@@ -4434,40 +4430,36 @@
       <c r="J100" t="n">
         <v>10</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
+      <c r="K100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>44100.56663462016</v>
+        <v>44100.62823132874</v>
       </c>
       <c r="B101" s="2" t="n">
-        <v>44100.56854659747</v>
+        <v>44100.63208025785</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>POINT (4.00482311611334 51.5012141033689)</t>
+          <t>POINT (4.13166341354231 51.5194499362428)</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>POINT (4.00461338253334 51.4997350921309)</t>
+          <t>POINT (4.13644117902828 51.5196719966841)</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>1.734183193260544</v>
+        <v>3.520729891498542</v>
       </c>
       <c r="F101" t="n">
-        <v>1344.019340451641</v>
+        <v>2727.298775179147</v>
       </c>
       <c r="G101" t="n">
-        <v>0.6390708388534938</v>
+        <v>1.289003850671483</v>
       </c>
       <c r="H101" t="n">
-        <v>19.14922473713535</v>
+        <v>38.65798601890555</v>
       </c>
       <c r="I101" t="n">
         <v>0</v>
@@ -4475,38 +4467,40 @@
       <c r="J101" t="n">
         <v>10</v>
       </c>
-      <c r="K101" t="n">
-        <v>4.8</v>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>44100.56854659747</v>
+        <v>44100.63208025785</v>
       </c>
       <c r="B102" s="2" t="n">
-        <v>44100.57152539599</v>
+        <v>44100.64135172852</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>POINT (4.00461338253334 51.4997350921309)</t>
+          <t>POINT (4.13644117902828 51.5196719966841)</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>POINT (4.004552683974264 51.49742214275099)</t>
+          <t>POINT (4.1478528804037 51.5207465272106)</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>2.701801082289497</v>
+        <v>8.48088988014333</v>
       </c>
       <c r="F102" t="n">
-        <v>2093.938473601716</v>
+        <v>6569.637914710115</v>
       </c>
       <c r="G102" t="n">
-        <v>0.9956516074713415</v>
+        <v>3.10500948671106</v>
       </c>
       <c r="H102" t="n">
-        <v>29.83387010060485</v>
+        <v>93.12106652155188</v>
       </c>
       <c r="I102" t="n">
         <v>0</v>
@@ -4522,32 +4516,32 @@
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>44100.57152539599</v>
+        <v>44100.64135172852</v>
       </c>
       <c r="B103" s="2" t="n">
-        <v>44100.57165413952</v>
+        <v>44100.64669117922</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>POINT (4.004552683974264 51.49742214275099)</t>
+          <t>POINT (4.1478528804037 51.5207465272106)</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>POINT (4.004550060584876 51.49732217716777)</t>
+          <t>POINT (4.15442084003053 51.5213823697844)</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.1167717140148051</v>
+        <v>4.88415431304939</v>
       </c>
       <c r="F103" t="n">
-        <v>90.49992102006031</v>
+        <v>3783.462090582199</v>
       </c>
       <c r="G103" t="n">
-        <v>0.04303201491839891</v>
+        <v>1.788178562448335</v>
       </c>
       <c r="H103" t="n">
-        <v>1.289418441184967</v>
+        <v>53.62853014859848</v>
       </c>
       <c r="I103" t="n">
         <v>0</v>
@@ -4555,38 +4549,36 @@
       <c r="J103" t="n">
         <v>10</v>
       </c>
-      <c r="K103" t="n">
-        <v>4.8</v>
-      </c>
+      <c r="K103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>44100.57165413952</v>
+        <v>44100.64669117922</v>
       </c>
       <c r="B104" s="2" t="n">
-        <v>44100.57466028699</v>
+        <v>44100.64936785868</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>POINT (4.004550060584876 51.49732217716777)</t>
+          <t>POINT (4.15442084003053 51.5213823697844)</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>POINT (4.00448880471598 51.4949879912145)</t>
+          <t>POINT (4.15745570231487 51.5205243986291)</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>2.7266068479421</v>
+        <v>2.448438282502796</v>
       </c>
       <c r="F104" t="n">
-        <v>2113.163333486668</v>
+        <v>1896.658628899002</v>
       </c>
       <c r="G104" t="n">
-        <v>1.004792880578635</v>
+        <v>0.8964182058893191</v>
       </c>
       <c r="H104" t="n">
-        <v>30.10778072427253</v>
+        <v>26.88411090049946</v>
       </c>
       <c r="I104" t="n">
         <v>0</v>
@@ -4602,32 +4594,32 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>44100.57466028699</v>
+        <v>44100.64936785868</v>
       </c>
       <c r="B105" s="2" t="n">
-        <v>44100.58220222829</v>
+        <v>44100.65168343043</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>POINT (4.00448880471598 51.4949879912145)</t>
+          <t>POINT (4.15745570231487 51.5205243986291)</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>POINT (4.00459248730018 51.489131461356)</t>
+          <t>POINT (4.15928008877698 51.5191322389496)</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>6.840618774443426</v>
+        <v>2.118122323581823</v>
       </c>
       <c r="F105" t="n">
-        <v>5301.587496285254</v>
+        <v>1640.782620889003</v>
       </c>
       <c r="G105" t="n">
-        <v>2.520863998915283</v>
+        <v>0.7754834695158365</v>
       </c>
       <c r="H105" t="n">
-        <v>75.53558746658646</v>
+        <v>23.25720680083716</v>
       </c>
       <c r="I105" t="n">
         <v>0</v>
@@ -4643,32 +4635,32 @@
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>44100.58220222829</v>
+        <v>44100.65168343043</v>
       </c>
       <c r="B106" s="2" t="n">
-        <v>44100.59511724286</v>
+        <v>44100.65735907064</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>POINT (4.00459248730018 51.489131461356)</t>
+          <t>POINT (4.15928008877698 51.5191322389496)</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>POINT (4.00514044121176 51.479107799445)</t>
+          <t>POINT (4.16235526778237 51.5151641970707)</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>11.71405181978086</v>
+        <v>5.191676844844832</v>
       </c>
       <c r="F106" t="n">
-        <v>9078.575009911916</v>
+        <v>4021.681394643501</v>
       </c>
       <c r="G106" t="n">
-        <v>4.316792454575058</v>
+        <v>1.900768207597757</v>
       </c>
       <c r="H106" t="n">
-        <v>129.3490859378273</v>
+        <v>57.00516003497388</v>
       </c>
       <c r="I106" t="n">
         <v>0</v>
@@ -4676,38 +4668,40 @@
       <c r="J106" t="n">
         <v>10</v>
       </c>
-      <c r="K106" t="n">
-        <v>4.8</v>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>44100.59511724286</v>
+        <v>44100.65735907064</v>
       </c>
       <c r="B107" s="2" t="n">
-        <v>44100.60216460839</v>
+        <v>44100.65825515905</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>POINT (4.00514044121176 51.479107799445)</t>
+          <t>POINT (4.16235526778237 51.5151641970707)</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>POINT (4.00544796116843 51.4736383428898)</t>
+          <t>POINT (4.16301868130238 51.5146048135391)</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>6.392033440571946</v>
+        <v>0.8196787156234961</v>
       </c>
       <c r="F107" t="n">
-        <v>4953.926783776139</v>
+        <v>634.9560534174976</v>
       </c>
       <c r="G107" t="n">
-        <v>2.355554009242793</v>
+        <v>0.3000994261533332</v>
       </c>
       <c r="H107" t="n">
-        <v>70.58221148563467</v>
+        <v>9.000158855595753</v>
       </c>
       <c r="I107" t="n">
         <v>0</v>
@@ -4723,32 +4717,32 @@
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>44100.60216460839</v>
+        <v>44100.65825515905</v>
       </c>
       <c r="B108" s="2" t="n">
-        <v>44100.60749566296</v>
+        <v>44100.66038538521</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>POINT (4.00544796116843 51.4736383428898)</t>
+          <t>POINT (4.16301868130238 51.5146048135391)</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>POINT (4.00595897849763 51.46951068115666)</t>
+          <t>POINT (4.16388199963191 51.513040695742)</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>4.835321645358238</v>
+        <v>1.948581201055258</v>
       </c>
       <c r="F108" t="n">
-        <v>3747.450577285013</v>
+        <v>1509.449258208373</v>
       </c>
       <c r="G108" t="n">
-        <v>1.78188387032339</v>
+        <v>0.7134113520623454</v>
       </c>
       <c r="H108" t="n">
-        <v>53.39266418284691</v>
+        <v>21.3956273741497</v>
       </c>
       <c r="I108" t="n">
         <v>0</v>
@@ -4764,32 +4758,32 @@
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>44100.60749566296</v>
+        <v>44100.66038538521</v>
       </c>
       <c r="B109" s="2" t="n">
-        <v>44100.60762383874</v>
+        <v>44100.66207205013</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>POINT (4.00595897849763 51.46951068115666)</t>
+          <t>POINT (4.16388199963191 51.513040695742)</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>POINT (4.00597126500701 51.46941143881848)</t>
+          <t>POINT (4.16534790837785 51.5121031534294)</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>0.1162567556922014</v>
+        <v>1.54284255098597</v>
       </c>
       <c r="F109" t="n">
-        <v>90.10082014979466</v>
+        <v>1195.147804280645</v>
       </c>
       <c r="G109" t="n">
-        <v>0.04284224526975466</v>
+        <v>0.564862982540841</v>
       </c>
       <c r="H109" t="n">
-        <v>1.283732153057071</v>
+        <v>16.94057412878537</v>
       </c>
       <c r="I109" t="n">
         <v>0</v>
@@ -4797,38 +4791,40 @@
       <c r="J109" t="n">
         <v>10</v>
       </c>
-      <c r="K109" t="n">
-        <v>4.8</v>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>44100.60762383874</v>
+        <v>44100.66207205013</v>
       </c>
       <c r="B110" s="2" t="n">
-        <v>44100.6077327005</v>
+        <v>44100.66815452045</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>POINT (4.00597126500701 51.46941143881848)</t>
+          <t>POINT (4.16534790837785 51.5121031534294)</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>POINT (4.005981700136667 51.46932715070748)</t>
+          <t>POINT (4.1724233102122 51.510424009286)</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.09873874011272761</v>
+        <v>5.563816448622184</v>
       </c>
       <c r="F110" t="n">
-        <v>76.52408177473143</v>
+        <v>4309.955677727459</v>
       </c>
       <c r="G110" t="n">
-        <v>0.03638661160261461</v>
+        <v>2.037015348370279</v>
       </c>
       <c r="H110" t="n">
-        <v>1.09029447035406</v>
+        <v>61.09129217647534</v>
       </c>
       <c r="I110" t="n">
         <v>0</v>
@@ -4836,38 +4832,36 @@
       <c r="J110" t="n">
         <v>10</v>
       </c>
-      <c r="K110" t="n">
-        <v>4.8</v>
-      </c>
+      <c r="K110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>44100.6077327005</v>
+        <v>44100.66815452045</v>
       </c>
       <c r="B111" s="2" t="n">
-        <v>44100.60786087628</v>
+        <v>44100.66905543306</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>POINT (4.005981700136667 51.46932715070748)</t>
+          <t>POINT (4.1724233102122 51.510424009286)</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>POINT (4.005993986646047 51.4692279083693)</t>
+          <t>POINT (4.173459437024155 51.51015669281915)</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>0.1162567555194477</v>
+        <v>0.8240915447881529</v>
       </c>
       <c r="F111" t="n">
-        <v>90.10082002353218</v>
+        <v>638.374408149332</v>
       </c>
       <c r="G111" t="n">
-        <v>0.04284224525472024</v>
+        <v>0.3017150441221765</v>
       </c>
       <c r="H111" t="n">
-        <v>1.283732152410206</v>
+        <v>9.048612190930058</v>
       </c>
       <c r="I111" t="n">
         <v>0</v>
@@ -4876,37 +4870,37 @@
         <v>10</v>
       </c>
       <c r="K111" t="n">
-        <v>4.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>44100.60786087628</v>
+        <v>44100.66905543306</v>
       </c>
       <c r="B112" s="2" t="n">
-        <v>44100.61007169095</v>
+        <v>44100.66939220678</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>POINT (4.005993986646047 51.4692279083693)</t>
+          <t>POINT (4.173459437024155 51.51015669281915)</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>POINT (4.00620590808444 51.4675161464354)</t>
+          <t>POINT (4.173846754383213 51.51005676652946)</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>2.005231779829179</v>
+        <v>0.3080569406458395</v>
       </c>
       <c r="F112" t="n">
-        <v>1554.086272314166</v>
+        <v>238.6332785623028</v>
       </c>
       <c r="G112" t="n">
-        <v>0.7389560465924805</v>
+        <v>0.1127853016728137</v>
       </c>
       <c r="H112" t="n">
-        <v>22.14220168623232</v>
+        <v>3.382497742448868</v>
       </c>
       <c r="I112" t="n">
         <v>0</v>
@@ -4914,40 +4908,38 @@
       <c r="J112" t="n">
         <v>10</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
+      <c r="K112" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44100.61007169095</v>
+        <v>44100.66939220678</v>
       </c>
       <c r="B113" s="2" t="n">
-        <v>44100.61563842568</v>
+        <v>44100.66953649408</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>POINT (4.00620590808444 51.4675161464354)</t>
+          <t>POINT (4.173846754383213 51.51005676652946)</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>POINT (4.00703931305038 51.4632245925606)</t>
+          <t>POINT (4.174012696359831 51.51001395418026)</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>5.049085991921999</v>
+        <v>0.1319838753319121</v>
       </c>
       <c r="F113" t="n">
-        <v>3913.121319039314</v>
+        <v>102.2400106435824</v>
       </c>
       <c r="G113" t="n">
-        <v>1.860659030912221</v>
+        <v>0.0483217199422129</v>
       </c>
       <c r="H113" t="n">
-        <v>55.75309617755484</v>
+        <v>1.44919689149575</v>
       </c>
       <c r="I113" t="n">
         <v>0</v>
@@ -4956,37 +4948,37 @@
         <v>10</v>
       </c>
       <c r="K113" t="n">
-        <v>4.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>44100.61563842568</v>
+        <v>44100.66953649408</v>
       </c>
       <c r="B114" s="2" t="n">
-        <v>44100.61833416695</v>
+        <v>44100.66962068767</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>POINT (4.007077769766 51.4632247650441)</t>
+          <t>POINT (4.174012696359831 51.51001395418026)</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>POINT (4.00782408176466 51.4611838755651)</t>
+          <t>POINT (4.174109525699595 51.50998897260784)</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>2.445065209451111</v>
+        <v>0.07701438820851468</v>
       </c>
       <c r="F114" t="n">
-        <v>1894.964120913144</v>
+        <v>59.65843821774006</v>
       </c>
       <c r="G114" t="n">
-        <v>0.9010408366859454</v>
+        <v>0.02819638158400356</v>
       </c>
       <c r="H114" t="n">
-        <v>26.99893725170027</v>
+        <v>0.845626119519282</v>
       </c>
       <c r="I114" t="n">
         <v>0</v>
@@ -4994,40 +4986,38 @@
       <c r="J114" t="n">
         <v>10</v>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
+      <c r="K114" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>44100.61833416695</v>
+        <v>44100.66962068767</v>
       </c>
       <c r="B115" s="2" t="n">
-        <v>44100.62375935472</v>
+        <v>44100.67262060999</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>POINT (4.00782408176466 51.4611838755651)</t>
+          <t>POINT (4.174109525699595 51.50998897260784)</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>POINT (4.00911825442341 51.45704908220779)</t>
+          <t>POINT (4.17755964573189 51.5090988557934)</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>4.920701436331074</v>
+        <v>2.744118134191439</v>
       </c>
       <c r="F115" t="n">
-        <v>3813.621262625284</v>
+        <v>2125.704117333955</v>
       </c>
       <c r="G115" t="n">
-        <v>1.813347521444295</v>
+        <v>1.004672028531056</v>
       </c>
       <c r="H115" t="n">
-        <v>54.33544624899218</v>
+        <v>30.13070691124264</v>
       </c>
       <c r="I115" t="n">
         <v>0</v>
@@ -5035,38 +5025,40 @@
       <c r="J115" t="n">
         <v>10</v>
       </c>
-      <c r="K115" t="n">
-        <v>4.8</v>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>44100.62375935472</v>
+        <v>44100.67262060999</v>
       </c>
       <c r="B116" s="2" t="n">
-        <v>44100.62381053418</v>
+        <v>44100.6742118926</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>POINT (4.00911825442341 51.45704908220779)</t>
+          <t>POINT (4.17755964573189 51.5090988557934)</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>POINT (4.00913046321188 51.4570100759615)</t>
+          <t>POINT (4.17953639624751 51.5091729988861)</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>0.04642029684282763</v>
+        <v>1.455593521158441</v>
       </c>
       <c r="F116" t="n">
-        <v>35.97646253778542</v>
+        <v>1127.56120169109</v>
       </c>
       <c r="G116" t="n">
-        <v>0.01710653048308485</v>
+        <v>0.5329195112385295</v>
       </c>
       <c r="H116" t="n">
-        <v>0.5125829209371929</v>
+        <v>15.98257057581914</v>
       </c>
       <c r="I116" t="n">
         <v>0</v>
@@ -5082,32 +5074,32 @@
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>44100.62381053418</v>
+        <v>44100.6742118926</v>
       </c>
       <c r="B117" s="2" t="n">
-        <v>44100.62388407332</v>
+        <v>44100.67620206127</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>POINT (4.00913046321188 51.4570100759615)</t>
+          <t>POINT (4.17953639624751 51.5091729988861)</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>POINT (4.009150080766985 51.4569542974622)</t>
+          <t>POINT (4.18184439930517 51.5097336944872)</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>0.06670076489501905</v>
+        <v>1.82046645196197</v>
       </c>
       <c r="F117" t="n">
-        <v>51.69414529912333</v>
+        <v>1410.20642816719</v>
       </c>
       <c r="G117" t="n">
-        <v>0.02458016746245896</v>
+        <v>0.6665061904245686</v>
       </c>
       <c r="H117" t="n">
-        <v>0.7365242206371533</v>
+        <v>19.98891390137148</v>
       </c>
       <c r="I117" t="n">
         <v>0</v>
@@ -5115,38 +5107,40 @@
       <c r="J117" t="n">
         <v>10</v>
       </c>
-      <c r="K117" t="n">
-        <v>4.8</v>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>44100.62388407332</v>
+        <v>44100.67620206127</v>
       </c>
       <c r="B118" s="2" t="n">
-        <v>44100.62562610097</v>
+        <v>44100.67861635847</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>POINT (4.009150080766985 51.4569542974622)</t>
+          <t>POINT (4.18184439930517 51.5097336944872)</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>POINT (4.009614789755068 51.4556329926499)</t>
+          <t>POINT (4.18457682100957 51.5105134558787)</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>1.580037098720772</v>
+        <v>2.20842943104841</v>
       </c>
       <c r="F118" t="n">
-        <v>1224.5536847944</v>
+        <v>1710.738133209694</v>
       </c>
       <c r="G118" t="n">
-        <v>0.5822658405905172</v>
+        <v>0.8085465590064661</v>
       </c>
       <c r="H118" t="n">
-        <v>17.44711033481343</v>
+        <v>24.2487883645945</v>
       </c>
       <c r="I118" t="n">
         <v>0</v>
@@ -5154,38 +5148,40 @@
       <c r="J118" t="n">
         <v>10</v>
       </c>
-      <c r="K118" t="n">
-        <v>4.8</v>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>44100.62562610097</v>
+        <v>44100.67861635847</v>
       </c>
       <c r="B119" s="2" t="n">
-        <v>44100.62612359502</v>
+        <v>44100.68042542834</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>POINT (4.009614789755068 51.4556329926499)</t>
+          <t>POINT (4.18457682100957 51.5105134558787)</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>POINT (4.009747502797199 51.45525565030076)</t>
+          <t>POINT (4.18681734620159 51.5103754505055)</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>0.4512322409379037</v>
+        <v>1.654809998890155</v>
       </c>
       <c r="F119" t="n">
-        <v>349.7121072086313</v>
+        <v>1281.882286431435</v>
       </c>
       <c r="G119" t="n">
-        <v>0.1662854117743733</v>
+        <v>0.6058563215688134</v>
       </c>
       <c r="H119" t="n">
-        <v>4.982603691960973</v>
+        <v>18.16998855013243</v>
       </c>
       <c r="I119" t="n">
         <v>0</v>
@@ -5193,38 +5189,40 @@
       <c r="J119" t="n">
         <v>10</v>
       </c>
-      <c r="K119" t="n">
-        <v>4.8</v>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>44100.62612359502</v>
+        <v>44100.68042542834</v>
       </c>
       <c r="B120" s="2" t="n">
-        <v>44100.62713497305</v>
+        <v>44100.6916516153</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>POINT (4.009747502797199 51.45525565030076)</t>
+          <t>POINT (4.18681734620159 51.5103754505055)</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>POINT (4.010017300984113 51.45448853442424)</t>
+          <t>POINT (4.19922485691811 51.5063685875487)</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>0.9173303382509906</v>
+        <v>10.26892698431746</v>
       </c>
       <c r="F120" t="n">
-        <v>710.9454877458741</v>
+        <v>7954.723267541933</v>
       </c>
       <c r="G120" t="n">
-        <v>0.3380491005382287</v>
+        <v>3.759642696924554</v>
       </c>
       <c r="H120" t="n">
-        <v>10.12935938398833</v>
+        <v>112.7539027435949</v>
       </c>
       <c r="I120" t="n">
         <v>0</v>
@@ -5233,37 +5231,37 @@
         <v>10</v>
       </c>
       <c r="K120" t="n">
-        <v>4.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>44100.62713497305</v>
+        <v>44100.6916516153</v>
       </c>
       <c r="B121" s="2" t="n">
-        <v>44100.62725934666</v>
+        <v>44100.69892465518</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>POINT (4.010017300984113 51.45448853442424)</t>
+          <t>POINT (4.19922485691811 51.5063685875487)</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>POINT (4.010050479244646 51.45439419883696)</t>
+          <t>POINT (4.20739704379769 51.5039415793045)</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0.1128081611920173</v>
+        <v>6.652865821881151</v>
       </c>
       <c r="F121" t="n">
-        <v>87.42810510745939</v>
+        <v>5153.577061227005</v>
       </c>
       <c r="G121" t="n">
-        <v>0.04157139054083419</v>
+        <v>2.435736318228881</v>
       </c>
       <c r="H121" t="n">
-        <v>1.245652047973303</v>
+        <v>73.04916931420006</v>
       </c>
       <c r="I121" t="n">
         <v>0</v>
@@ -5271,38 +5269,40 @@
       <c r="J121" t="n">
         <v>10</v>
       </c>
-      <c r="K121" t="n">
-        <v>4.8</v>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>44100.62725934666</v>
+        <v>44100.69892465518</v>
       </c>
       <c r="B122" s="2" t="n">
-        <v>44100.62735150801</v>
+        <v>44100.70244901737</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>POINT (4.010050479244646 51.45439419883696)</t>
+          <t>POINT (4.20739704379769 51.5039415793045)</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>POINT (4.01007506446769 51.4543242957915)</t>
+          <t>POINT (4.21026814694432 51.5060104715131)</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>0.08359129257540784</v>
+        <v>3.223838879538069</v>
       </c>
       <c r="F122" t="n">
-        <v>64.78457076554301</v>
+        <v>2497.315073396114</v>
       </c>
       <c r="G122" t="n">
-        <v>0.03080456376804752</v>
+        <v>1.180306600284225</v>
       </c>
       <c r="H122" t="n">
-        <v>0.9230330656782649</v>
+        <v>35.39809134736284</v>
       </c>
       <c r="I122" t="n">
         <v>0</v>
@@ -5318,32 +5318,32 @@
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>44100.62735150801</v>
+        <v>44100.70244901737</v>
       </c>
       <c r="B123" s="2" t="n">
-        <v>44100.62752002849</v>
+        <v>44100.70622251128</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>POINT (4.01007506446769 51.4543242957915)</t>
+          <t>POINT (4.21026814694432 51.5060104715131)</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>POINT (4.0101364036441 51.454199162881)</t>
+          <t>POINT (4.21156096017467 51.5088276240167)</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>0.1528498223355888</v>
+        <v>3.451727074758937</v>
       </c>
       <c r="F123" t="n">
-        <v>118.4610243871923</v>
+        <v>2673.846421983765</v>
       </c>
       <c r="G123" t="n">
-        <v>0.05632730468353251</v>
+        <v>1.263740652474688</v>
       </c>
       <c r="H123" t="n">
-        <v>1.687800708885804</v>
+        <v>37.9003277998554</v>
       </c>
       <c r="I123" t="n">
         <v>0</v>
@@ -5351,38 +5351,40 @@
       <c r="J123" t="n">
         <v>10</v>
       </c>
-      <c r="K123" t="n">
-        <v>4.8</v>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>44100.62752002849</v>
+        <v>44100.70622251128</v>
       </c>
       <c r="B124" s="2" t="n">
-        <v>44100.63107497147</v>
+        <v>44100.71106664356</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>POINT (4.0101364036441 51.454199162881)</t>
+          <t>POINT (4.21156096017467 51.5088276240167)</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>POINT (4.01139622477123 51.4515530514673)</t>
+          <t>POINT (4.21411639050789 51.5122347688903)</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>3.22437005463868</v>
+        <v>4.431071821121071</v>
       </c>
       <c r="F124" t="n">
-        <v>2498.937673342617</v>
+        <v>3432.486195465627</v>
       </c>
       <c r="G124" t="n">
-        <v>1.188225605587004</v>
+        <v>1.622296744259283</v>
       </c>
       <c r="H124" t="n">
-        <v>35.60418935949204</v>
+        <v>48.65363654644972</v>
       </c>
       <c r="I124" t="n">
         <v>0</v>
@@ -5390,38 +5392,40 @@
       <c r="J124" t="n">
         <v>10</v>
       </c>
-      <c r="K124" t="n">
-        <v>4.8</v>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>44100.63107497147</v>
+        <v>44100.71106664356</v>
       </c>
       <c r="B125" s="2" t="n">
-        <v>44100.63392552155</v>
+        <v>44100.71633170145</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>POINT (4.01139622477123 51.4515530514673)</t>
+          <t>POINT (4.21411639050789 51.5122347688903)</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>POINT (4.012424164789 51.4494345917777)</t>
+          <t>POINT (4.21832420191664 51.5153691585079)</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>2.585478411088143</v>
+        <v>4.816104983308227</v>
       </c>
       <c r="F125" t="n">
-        <v>2003.786567882995</v>
+        <v>3730.748346812062</v>
       </c>
       <c r="G125" t="n">
-        <v>0.9527850713530822</v>
+        <v>1.763264453996439</v>
       </c>
       <c r="H125" t="n">
-        <v>28.54941009276589</v>
+        <v>52.8813413343271</v>
       </c>
       <c r="I125" t="n">
         <v>0</v>
@@ -5437,32 +5441,32 @@
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>44100.63392552155</v>
+        <v>44100.71633170145</v>
       </c>
       <c r="B126" s="2" t="n">
-        <v>44100.63643388361</v>
+        <v>44100.72302200154</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>POINT (4.012424164789 51.4494345917777)</t>
+          <t>POINT (4.21832420191664 51.5153691585079)</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>POINT (4.01312883607665 51.4475370610685)</t>
+          <t>POINT (4.22314317985118 51.5196063551146)</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>2.275110337355795</v>
+        <v>6.119816410866855</v>
       </c>
       <c r="F126" t="n">
-        <v>1763.246413037955</v>
+        <v>4740.655578767815</v>
       </c>
       <c r="G126" t="n">
-        <v>0.8384100811418495</v>
+        <v>2.240577141890595</v>
       </c>
       <c r="H126" t="n">
-        <v>25.12225889460187</v>
+        <v>67.19623047081653</v>
       </c>
       <c r="I126" t="n">
         <v>0</v>
@@ -5470,40 +5474,38 @@
       <c r="J126" t="n">
         <v>10</v>
       </c>
-      <c r="K126" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
+      <c r="K126" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>44100.63643388361</v>
+        <v>44100.72302200154</v>
       </c>
       <c r="B127" s="2" t="n">
-        <v>44100.63937753432</v>
+        <v>44100.72745199272</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>POINT (4.01312883607665 51.4475370610685)</t>
+          <t>POINT (4.22314317985118 51.5196063551146)</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>POINT (4.01338463474318 51.4452566710847)</t>
+          <t>POINT (4.22123751438415 51.5163781245686)</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>2.669921641889514</v>
+        <v>4.052244644883182</v>
       </c>
       <c r="F127" t="n">
-        <v>2069.23140424537</v>
+        <v>3139.031450084748</v>
       </c>
       <c r="G127" t="n">
-        <v>0.9839035864894087</v>
+        <v>1.483601159923975</v>
       </c>
       <c r="H127" t="n">
-        <v>29.48185044865581</v>
+        <v>44.49407413993291</v>
       </c>
       <c r="I127" t="n">
         <v>0</v>
@@ -5511,40 +5513,38 @@
       <c r="J127" t="n">
         <v>10</v>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
+      <c r="K127" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>44100.63937753432</v>
+        <v>44100.72745199272</v>
       </c>
       <c r="B128" s="2" t="n">
-        <v>44100.6407440537</v>
+        <v>44100.72966037778</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>POINT (4.01338463474318 51.4452566710847)</t>
+          <t>POINT (4.22123751438415 51.5163781245686)</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>POINT (4.01347413381982 51.4441969316557)</t>
+          <t>POINT (4.22050187857941 51.5147257140302)</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>1.239447220215981</v>
+        <v>2.020075471385661</v>
       </c>
       <c r="F128" t="n">
-        <v>960.591154329547</v>
+        <v>1564.831591381081</v>
       </c>
       <c r="G128" t="n">
-        <v>0.456753691176584</v>
+        <v>0.7395867169232641</v>
       </c>
       <c r="H128" t="n">
-        <v>13.68624344932914</v>
+        <v>22.18064201061336</v>
       </c>
       <c r="I128" t="n">
         <v>0</v>
@@ -5552,887 +5552,7 @@
       <c r="J128" t="n">
         <v>10</v>
       </c>
-      <c r="K128" t="n">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="2" t="n">
-        <v>44100.6407440537</v>
-      </c>
-      <c r="B129" s="2" t="n">
-        <v>44100.64218542629</v>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>POINT (4.01347413381982 51.4441969316557)</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>POINT (4.01314768372824 51.4430963347628)</t>
-        </is>
-      </c>
-      <c r="E129" t="n">
-        <v>1.307339840066451</v>
-      </c>
-      <c r="F129" t="n">
-        <v>1013.209006151613</v>
-      </c>
-      <c r="G129" t="n">
-        <v>0.4817730747089835</v>
-      </c>
-      <c r="H129" t="n">
-        <v>14.43592841000587</v>
-      </c>
-      <c r="I129" t="n">
-        <v>0</v>
-      </c>
-      <c r="J129" t="n">
-        <v>10</v>
-      </c>
-      <c r="K129" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="2" t="n">
-        <v>44100.64218542629</v>
-      </c>
-      <c r="B130" s="2" t="n">
-        <v>44100.64453232841</v>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>POINT (4.01314768372824 51.4430963347628)</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>POINT (4.01235185555159 51.4413429421687)</t>
-        </is>
-      </c>
-      <c r="E130" t="n">
-        <v>2.12866450070194</v>
-      </c>
-      <c r="F130" t="n">
-        <v>1649.748578643081</v>
-      </c>
-      <c r="G130" t="n">
-        <v>0.7844427352468145</v>
-      </c>
-      <c r="H130" t="n">
-        <v>23.50517238188793</v>
-      </c>
-      <c r="I130" t="n">
-        <v>0</v>
-      </c>
-      <c r="J130" t="n">
-        <v>10</v>
-      </c>
-      <c r="K130" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="2" t="n">
-        <v>44100.64453232841</v>
-      </c>
-      <c r="B131" s="2" t="n">
-        <v>44100.64679578145</v>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>POINT (4.01235185555159 51.4413429421687)</t>
-        </is>
-      </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>POINT (4.01123540415855 51.4397295986581)</t>
-        </is>
-      </c>
-      <c r="E131" t="n">
-        <v>2.052975324576845</v>
-      </c>
-      <c r="F131" t="n">
-        <v>1591.088272877131</v>
-      </c>
-      <c r="G131" t="n">
-        <v>0.756550212608865</v>
-      </c>
-      <c r="H131" t="n">
-        <v>22.66939619880382</v>
-      </c>
-      <c r="I131" t="n">
-        <v>0</v>
-      </c>
-      <c r="J131" t="n">
-        <v>10</v>
-      </c>
-      <c r="K131" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="2" t="n">
-        <v>44100.64679578145</v>
-      </c>
-      <c r="B132" s="2" t="n">
-        <v>44100.64944883241</v>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>POINT (4.01123540415855 51.4397295986581)</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>POINT (4.00967926827773 51.4379132772321)</t>
-        </is>
-      </c>
-      <c r="E132" t="n">
-        <v>2.406344667249623</v>
-      </c>
-      <c r="F132" t="n">
-        <v>1864.955089586548</v>
-      </c>
-      <c r="G132" t="n">
-        <v>0.8867717729351322</v>
-      </c>
-      <c r="H132" t="n">
-        <v>26.57137665869193</v>
-      </c>
-      <c r="I132" t="n">
-        <v>0</v>
-      </c>
-      <c r="J132" t="n">
-        <v>10</v>
-      </c>
-      <c r="K132" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="2" t="n">
-        <v>44100.64944883241</v>
-      </c>
-      <c r="B133" s="2" t="n">
-        <v>44100.6524694718</v>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>POINT (4.00967926827773 51.4379132772321)</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>POINT (4.00791520113023 51.4358427614001)</t>
-        </is>
-      </c>
-      <c r="E133" t="n">
-        <v>2.73975117088265</v>
-      </c>
-      <c r="F133" t="n">
-        <v>2123.350391167036</v>
-      </c>
-      <c r="G133" t="n">
-        <v>1.00963674789416</v>
-      </c>
-      <c r="H133" t="n">
-        <v>30.25292316933247</v>
-      </c>
-      <c r="I133" t="n">
-        <v>0</v>
-      </c>
-      <c r="J133" t="n">
-        <v>10</v>
-      </c>
-      <c r="K133" t="inlineStr"/>
-    </row>
-    <row r="134">
-      <c r="A134" s="2" t="n">
-        <v>44100.6524694718</v>
-      </c>
-      <c r="B134" s="2" t="n">
-        <v>44100.66036736943</v>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>POINT (4.00791520113023 51.4358427614001)</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>POINT (4.01655675552499 51.4329369466678)</t>
-        </is>
-      </c>
-      <c r="E134" t="n">
-        <v>7.163474861175327</v>
-      </c>
-      <c r="F134" t="n">
-        <v>5551.806058147121</v>
-      </c>
-      <c r="G134" t="n">
-        <v>2.639840996365808</v>
-      </c>
-      <c r="H134" t="n">
-        <v>79.10063397696632</v>
-      </c>
-      <c r="I134" t="n">
-        <v>0</v>
-      </c>
-      <c r="J134" t="n">
-        <v>10</v>
-      </c>
-      <c r="K134" t="inlineStr"/>
-    </row>
-    <row r="135">
-      <c r="A135" s="2" t="n">
-        <v>44100.66036736943</v>
-      </c>
-      <c r="B135" s="2" t="n">
-        <v>44100.66871953757</v>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>POINT (4.01655675552499 51.4329369466678)</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>POINT (4.02422713226244 51.4285687560799)</t>
-        </is>
-      </c>
-      <c r="E135" t="n">
-        <v>7.575502899401494</v>
-      </c>
-      <c r="F135" t="n">
-        <v>5871.134289750485</v>
-      </c>
-      <c r="G135" t="n">
-        <v>2.791679110293317</v>
-      </c>
-      <c r="H135" t="n">
-        <v>83.65033643345461</v>
-      </c>
-      <c r="I135" t="n">
-        <v>0</v>
-      </c>
-      <c r="J135" t="n">
-        <v>10</v>
-      </c>
-      <c r="K135" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="2" t="n">
-        <v>44100.66871953757</v>
-      </c>
-      <c r="B136" s="2" t="n">
-        <v>44100.67726348315</v>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>POINT (4.02422713226244 51.4285687560799)</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>POINT (4.02919015197277 51.4227037971299)</t>
-        </is>
-      </c>
-      <c r="E136" t="n">
-        <v>7.749447025714298</v>
-      </c>
-      <c r="F136" t="n">
-        <v>6005.943732402564</v>
-      </c>
-      <c r="G136" t="n">
-        <v>2.855779960760313</v>
-      </c>
-      <c r="H136" t="n">
-        <v>85.5710649639044</v>
-      </c>
-      <c r="I136" t="n">
-        <v>0</v>
-      </c>
-      <c r="J136" t="n">
-        <v>10</v>
-      </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="2" t="n">
-        <v>44100.67726348315</v>
-      </c>
-      <c r="B137" s="2" t="n">
-        <v>44100.68470105426</v>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>POINT (4.02919015197277 51.4227037971299)</t>
-        </is>
-      </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>POINT (4.03159701157359 51.4171273758914)</t>
-        </is>
-      </c>
-      <c r="E137" t="n">
-        <v>6.745953936773534</v>
-      </c>
-      <c r="F137" t="n">
-        <v>5228.220753265869</v>
-      </c>
-      <c r="G137" t="n">
-        <v>2.485978678003905</v>
-      </c>
-      <c r="H137" t="n">
-        <v>74.49027791786274</v>
-      </c>
-      <c r="I137" t="n">
-        <v>0</v>
-      </c>
-      <c r="J137" t="n">
-        <v>10</v>
-      </c>
-      <c r="K137" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="2" t="n">
-        <v>44100.68470105426</v>
-      </c>
-      <c r="B138" s="2" t="n">
-        <v>44100.68666648037</v>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>POINT (4.03155652968014 51.4171249453695)</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>POINT (4.03399701530433 51.4171568523138)</t>
-        </is>
-      </c>
-      <c r="E138" t="n">
-        <v>1.782661814318889</v>
-      </c>
-      <c r="F138" t="n">
-        <v>1381.591036798483</v>
-      </c>
-      <c r="G138" t="n">
-        <v>0.6569358910814821</v>
-      </c>
-      <c r="H138" t="n">
-        <v>19.68453612801372</v>
-      </c>
-      <c r="I138" t="n">
-        <v>0</v>
-      </c>
-      <c r="J138" t="n">
-        <v>10</v>
-      </c>
-      <c r="K138" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="2" t="n">
-        <v>44100.68666648037</v>
-      </c>
-      <c r="B139" s="2" t="n">
-        <v>44100.6934308855</v>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>POINT (4.03399701530433 51.4171568523138)</t>
-        </is>
-      </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>POINT (4.04239677466316 51.4170580077231)</t>
-        </is>
-      </c>
-      <c r="E139" t="n">
-        <v>6.135385427382354</v>
-      </c>
-      <c r="F139" t="n">
-        <v>4755.020523546495</v>
-      </c>
-      <c r="G139" t="n">
-        <v>2.260975614980055</v>
-      </c>
-      <c r="H139" t="n">
-        <v>67.74824877623192</v>
-      </c>
-      <c r="I139" t="n">
-        <v>0</v>
-      </c>
-      <c r="J139" t="n">
-        <v>10</v>
-      </c>
-      <c r="K139" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="2" t="n">
-        <v>44100.6934308855</v>
-      </c>
-      <c r="B140" s="2" t="n">
-        <v>44100.70016255356</v>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>POINT (4.04239677466316 51.4170580077231)</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>POINT (4.04979778603265 51.4146265214129)</t>
-        </is>
-      </c>
-      <c r="E140" t="n">
-        <v>6.105692563353643</v>
-      </c>
-      <c r="F140" t="n">
-        <v>4732.008085422875</v>
-      </c>
-      <c r="G140" t="n">
-        <v>2.25003337832875</v>
-      </c>
-      <c r="H140" t="n">
-        <v>67.42037377872869</v>
-      </c>
-      <c r="I140" t="n">
-        <v>0</v>
-      </c>
-      <c r="J140" t="n">
-        <v>10</v>
-      </c>
-      <c r="K140" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="2" t="n">
-        <v>44100.70016255356</v>
-      </c>
-      <c r="B141" s="2" t="n">
-        <v>44100.7436967234</v>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>POINT (4.04979778603265 51.4146265214129)</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>POINT (4.08774409187943 51.3905505521455)</t>
-        </is>
-      </c>
-      <c r="E141" t="n">
-        <v>39.48594240280404</v>
-      </c>
-      <c r="F141" t="n">
-        <v>30602.22845668575</v>
-      </c>
-      <c r="G141" t="n">
-        <v>14.55112380054189</v>
-      </c>
-      <c r="H141" t="n">
-        <v>436.0122898564441</v>
-      </c>
-      <c r="I141" t="n">
-        <v>0</v>
-      </c>
-      <c r="J141" t="n">
-        <v>10</v>
-      </c>
-      <c r="K141" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="2" t="n">
-        <v>44100.7436967234</v>
-      </c>
-      <c r="B142" s="2" t="n">
-        <v>44100.76459109404</v>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>POINT (4.08774409187943 51.3905505521455)</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>POINT (4.10143801222551 51.3767712316792)</t>
-        </is>
-      </c>
-      <c r="E142" t="n">
-        <v>18.95141031497851</v>
-      </c>
-      <c r="F142" t="n">
-        <v>14687.64205036423</v>
-      </c>
-      <c r="G142" t="n">
-        <v>6.983860607005</v>
-      </c>
-      <c r="H142" t="n">
-        <v>209.2655589392347</v>
-      </c>
-      <c r="I142" t="n">
-        <v>0</v>
-      </c>
-      <c r="J142" t="n">
-        <v>10</v>
-      </c>
-      <c r="K142" t="inlineStr"/>
-    </row>
-    <row r="143">
-      <c r="A143" s="2" t="n">
-        <v>44100.76459109404</v>
-      </c>
-      <c r="B143" s="2" t="n">
-        <v>44100.77590991986</v>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>POINT (4.10143801222551 51.3767712316792)</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>POINT (4.11309261130701 51.3718661585277)</t>
-        </is>
-      </c>
-      <c r="E143" t="n">
-        <v>10.26629211072801</v>
-      </c>
-      <c r="F143" t="n">
-        <v>7956.538389544352</v>
-      </c>
-      <c r="G143" t="n">
-        <v>3.783272688537103</v>
-      </c>
-      <c r="H143" t="n">
-        <v>113.3626110735194</v>
-      </c>
-      <c r="I143" t="n">
-        <v>0</v>
-      </c>
-      <c r="J143" t="n">
-        <v>10</v>
-      </c>
-      <c r="K143" t="inlineStr"/>
-    </row>
-    <row r="144">
-      <c r="A144" s="2" t="n">
-        <v>44100.77590991986</v>
-      </c>
-      <c r="B144" s="2" t="n">
-        <v>44100.78266241977</v>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>POINT (4.11309261130701 51.3718661585277)</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>POINT (4.12117307341129 51.370480906923)</t>
-        </is>
-      </c>
-      <c r="E144" t="n">
-        <v>6.124587269973232</v>
-      </c>
-      <c r="F144" t="n">
-        <v>4746.651781148798</v>
-      </c>
-      <c r="G144" t="n">
-        <v>2.256996342409238</v>
-      </c>
-      <c r="H144" t="n">
-        <v>67.62901319237004</v>
-      </c>
-      <c r="I144" t="n">
-        <v>0</v>
-      </c>
-      <c r="J144" t="n">
-        <v>10</v>
-      </c>
-      <c r="K144" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="2" t="n">
-        <v>44100.78266241977</v>
-      </c>
-      <c r="B145" s="2" t="n">
-        <v>44100.78550946504</v>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>POINT (4.12121289886391 51.3704872312544)</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>POINT (4.12472512662219 51.3707231044718)</t>
-        </is>
-      </c>
-      <c r="E145" t="n">
-        <v>2.582299517974748</v>
-      </c>
-      <c r="F145" t="n">
-        <v>2001.322875570695</v>
-      </c>
-      <c r="G145" t="n">
-        <v>0.9516136047273753</v>
-      </c>
-      <c r="H145" t="n">
-        <v>28.51430807190326</v>
-      </c>
-      <c r="I145" t="n">
-        <v>0</v>
-      </c>
-      <c r="J145" t="n">
-        <v>10</v>
-      </c>
-      <c r="K145" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="2" t="n">
-        <v>44100.78550946504</v>
-      </c>
-      <c r="B146" s="2" t="n">
-        <v>44100.7889443004</v>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>POINT (4.12472512662219 51.3707231044718)</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>POINT (4.12890454448905 51.3712447558052)</t>
-        </is>
-      </c>
-      <c r="E146" t="n">
-        <v>3.115431191979248</v>
-      </c>
-      <c r="F146" t="n">
-        <v>2414.508335806071</v>
-      </c>
-      <c r="G146" t="n">
-        <v>1.148080106802092</v>
-      </c>
-      <c r="H146" t="n">
-        <v>34.40126296500705</v>
-      </c>
-      <c r="I146" t="n">
-        <v>0</v>
-      </c>
-      <c r="J146" t="n">
-        <v>10</v>
-      </c>
-      <c r="K146" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="2" t="n">
-        <v>44100.7889443004</v>
-      </c>
-      <c r="B147" s="2" t="n">
-        <v>44100.79494885968</v>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>POINT (4.12890454448905 51.3712447558052)</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>POINT (4.13615707644801 51.3723116945366)</t>
-        </is>
-      </c>
-      <c r="E147" t="n">
-        <v>5.446197386172887</v>
-      </c>
-      <c r="F147" t="n">
-        <v>4220.888916088127</v>
-      </c>
-      <c r="G147" t="n">
-        <v>2.007000151687432</v>
-      </c>
-      <c r="H147" t="n">
-        <v>60.13808582065291</v>
-      </c>
-      <c r="I147" t="n">
-        <v>0</v>
-      </c>
-      <c r="J147" t="n">
-        <v>10</v>
-      </c>
-      <c r="K147" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="2" t="n">
-        <v>44100.79494885968</v>
-      </c>
-      <c r="B148" s="2" t="n">
-        <v>44100.80238109132</v>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>POINT (4.13615707644801 51.3723116945366)</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>POINT (4.14495101587775 51.3740494583674)</t>
-        </is>
-      </c>
-      <c r="E148" t="n">
-        <v>6.741110983895317</v>
-      </c>
-      <c r="F148" t="n">
-        <v>5224.467388386348</v>
-      </c>
-      <c r="G148" t="n">
-        <v>2.484193982068057</v>
-      </c>
-      <c r="H148" t="n">
-        <v>74.43680099187236</v>
-      </c>
-      <c r="I148" t="n">
-        <v>0</v>
-      </c>
-      <c r="J148" t="n">
-        <v>10</v>
-      </c>
-      <c r="K148" t="inlineStr"/>
-    </row>
-    <row r="149">
-      <c r="A149" s="2" t="n">
-        <v>44100.80238109132</v>
-      </c>
-      <c r="B149" s="2" t="n">
-        <v>44100.80687873907</v>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>POINT (4.14495101587775 51.3740494583674)</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>POINT (4.14974037798965 51.3758425128673)</t>
-        </is>
-      </c>
-      <c r="E149" t="n">
-        <v>4.079413040303621</v>
-      </c>
-      <c r="F149" t="n">
-        <v>3161.609480032716</v>
-      </c>
-      <c r="G149" t="n">
-        <v>1.503320943402737</v>
-      </c>
-      <c r="H149" t="n">
-        <v>45.04575838301167</v>
-      </c>
-      <c r="I149" t="n">
-        <v>0</v>
-      </c>
-      <c r="J149" t="n">
-        <v>10</v>
-      </c>
-      <c r="K149" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="2" t="n">
-        <v>44100.80687873907</v>
-      </c>
-      <c r="B150" s="2" t="n">
-        <v>44100.81107049937</v>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>POINT (4.14974037798965 51.3758425128673)</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>POINT (4.15338912378385 51.3781625305816)</t>
-        </is>
-      </c>
-      <c r="E150" t="n">
-        <v>3.801969956116368</v>
-      </c>
-      <c r="F150" t="n">
-        <v>2946.586711662684</v>
-      </c>
-      <c r="G150" t="n">
-        <v>1.401079273909247</v>
-      </c>
-      <c r="H150" t="n">
-        <v>41.98217202123068</v>
-      </c>
-      <c r="I150" t="n">
-        <v>0</v>
-      </c>
-      <c r="J150" t="n">
-        <v>10</v>
-      </c>
-      <c r="K150" t="inlineStr">
+      <c r="K128" t="inlineStr">
         <is>
           <t>'NoneType' object is not subscriptable</t>
         </is>

</xml_diff>

<commit_message>
Bug in dijkstra path removed / Created locks on the edges in Example 14 (not working yet)
</commit_message>
<xml_diff>
--- a/notebooks/Data Zuid_Beveland.xlsx
+++ b/notebooks/Data Zuid_Beveland.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,29 +500,29 @@
         <v>44100</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44100.00009965996</v>
+        <v>44100.00141703648</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>POINT (4.201416987493968 51.58410292465058)</t>
+          <t>POINT (4.22456143757696 51.5221824639149)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>POINT (4.201336029861413 51.58416162611335)</t>
+          <t>POINT (4.22514008092064 51.5232220043962)</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.09076967773911737</v>
+        <v>1.283496169009298</v>
       </c>
       <c r="F2" t="n">
-        <v>70.33122155187218</v>
+        <v>994.8078202114579</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03334331750537183</v>
+        <v>0.4734840533809876</v>
       </c>
       <c r="H2" t="n">
-        <v>0.999535107604371</v>
+        <v>14.18554494212907</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -530,38 +530,40 @@
       <c r="J2" t="n">
         <v>10</v>
       </c>
-      <c r="K2" t="n">
-        <v>4.3</v>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44100.00009965996</v>
+        <v>44100.00141703648</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44100.00031463027</v>
+        <v>44100.005461837</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>POINT (4.201336029861413 51.58416162611335)</t>
+          <t>POINT (4.22514008092064 51.5232220043962)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>POINT (4.20116140102169 51.5842882475079)</t>
+          <t>POINT (4.22672112709352 51.5262042274209)</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.1957936481081705</v>
+        <v>3.663621957717715</v>
       </c>
       <c r="F3" t="n">
-        <v>151.7071205924036</v>
+        <v>2839.587574949268</v>
       </c>
       <c r="G3" t="n">
-        <v>0.07192280460198451</v>
+        <v>1.351516753703045</v>
       </c>
       <c r="H3" t="n">
-        <v>2.156035259347238</v>
+        <v>40.49133547604553</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -569,40 +571,36 @@
       <c r="J3" t="n">
         <v>10</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
-      </c>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44100.00031463027</v>
+        <v>44100.005461837</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44100.0026669078</v>
+        <v>44100.02005154493</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>POINT (4.20116140102169 51.5842882475079)</t>
+          <t>POINT (4.22672112709352 51.5262042274209)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>POINT (4.19934887369148 51.5857241535032)</t>
+          <t>POINT (4.232825345579756 51.53687532596246)</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2.142440021991124</v>
+        <v>13.21478625585007</v>
       </c>
       <c r="F4" t="n">
-        <v>1660.030393591016</v>
+        <v>10242.47132768802</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7870035430923328</v>
+        <v>4.87495850432483</v>
       </c>
       <c r="H4" t="n">
-        <v>23.59206371289764</v>
+        <v>146.0533727699051</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -618,32 +616,32 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44100.0026669078</v>
+        <v>44100.02005154493</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44100.00503643882</v>
+        <v>44100.02007196246</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>POINT (4.19934887369148 51.5857241535032)</t>
+          <t>POINT (4.232825345579756 51.53687532596246)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>POINT (4.19763109913537 51.5872210992283)</t>
+          <t>POINT (4.23283388821669 51.5368902597858)</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2.158154390451413</v>
+        <v>0.01849339338902203</v>
       </c>
       <c r="F5" t="n">
-        <v>1672.206384014964</v>
+        <v>14.33379607637012</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7927760562510409</v>
+        <v>0.006822246129791094</v>
       </c>
       <c r="H5" t="n">
-        <v>23.76510676978024</v>
+        <v>0.2043939569342471</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -659,32 +657,32 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44100.00503643882</v>
+        <v>44100.02007196246</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44100.0080964992</v>
+        <v>44100.02017324961</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>POINT (4.19763109913537 51.5872210992283)</t>
+          <t>POINT (4.23283388821669 51.5368902597858)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>POINT (4.19562926259692 51.5892439548483)</t>
+          <t>POINT (4.232866956880075 51.5369661646866)</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2.787084318732481</v>
+        <v>0.09174193730068879</v>
       </c>
       <c r="F6" t="n">
-        <v>2159.521214677369</v>
+        <v>71.10702695701025</v>
       </c>
       <c r="G6" t="n">
-        <v>1.023807066546209</v>
+        <v>0.03384376636271021</v>
       </c>
       <c r="H6" t="n">
-        <v>30.69074053737102</v>
+        <v>1.013956573875512</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -692,40 +690,38 @@
       <c r="J6" t="n">
         <v>10</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
+      <c r="K6" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44100.0080964992</v>
+        <v>44100.02017324961</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44100.0116341409</v>
+        <v>44100.02308820059</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>POINT (4.19562926259692 51.5892439548483)</t>
+          <t>POINT (4.232866956880075 51.5369661646866)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>POINT (4.19369271232264 51.5917121585537)</t>
+          <t>POINT (4.23381864402466 51.5391506411942)</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3.222062468346308</v>
+        <v>2.640248480742988</v>
       </c>
       <c r="F7" t="n">
-        <v>2496.556063550779</v>
+        <v>2046.394761036335</v>
       </c>
       <c r="G7" t="n">
-        <v>1.183591864346118</v>
+        <v>0.9739924306634957</v>
       </c>
       <c r="H7" t="n">
-        <v>35.48062129705323</v>
+        <v>29.18073649706297</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -741,32 +737,32 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44100.0116341409</v>
+        <v>44100.02308820059</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44100.01444897324</v>
+        <v>44100.0261023963</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>POINT (4.19369271232264 51.5917121585537)</t>
+          <t>POINT (4.23381864402466 51.5391506411942)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>POINT (4.19244257593752 51.5937546589974)</t>
+          <t>POINT (4.23494916828471 51.5413826869409)</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2.563732113042757</v>
+        <v>2.730140464819426</v>
       </c>
       <c r="F8" t="n">
-        <v>1986.460850736517</v>
+        <v>2116.067932558223</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9417609063392809</v>
+        <v>1.007153745826535</v>
       </c>
       <c r="H8" t="n">
-        <v>28.23123669405758</v>
+        <v>30.17424688722292</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -782,32 +778,32 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44100.01444897324</v>
+        <v>44100.0261023963</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44100.01678086176</v>
+        <v>44100.02966374232</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>POINT (4.19244257593752 51.5937546589974)</t>
+          <t>POINT (4.23494916828471 51.5413826869409)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>POINT (4.19160568283927 51.5954888733602)</t>
+          <t>POINT (4.23606856568404 51.5440587855062)</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2.123869831305974</v>
+        <v>3.225727798680138</v>
       </c>
       <c r="F9" t="n">
-        <v>1645.641621576488</v>
+        <v>2500.186067969634</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7801819722573957</v>
+        <v>1.189976807421207</v>
       </c>
       <c r="H9" t="n">
-        <v>23.38757297785374</v>
+        <v>35.65161141280787</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -823,32 +819,32 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44100.01678086176</v>
+        <v>44100.02966374232</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44100.01972497862</v>
+        <v>44100.03271985429</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>POINT (4.19160568283927 51.5954888733602)</t>
+          <t>POINT (4.23606856568404 51.5440587855062)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>POINT (4.19087118673537 51.5977289297391)</t>
+          <t>POINT (4.2362459507422 51.5464294871925)</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2.681483669928345</v>
+        <v>2.768106582661822</v>
       </c>
       <c r="F10" t="n">
-        <v>2077.698486937112</v>
+        <v>2145.494581365564</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9850157426140526</v>
+        <v>1.021159515614338</v>
       </c>
       <c r="H10" t="n">
-        <v>29.52789013657621</v>
+        <v>30.59385864523661</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -856,38 +852,40 @@
       <c r="J10" t="n">
         <v>10</v>
       </c>
-      <c r="K10" t="n">
-        <v>4.3</v>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44100.01972497862</v>
+        <v>44100.03271985429</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44100.02224001205</v>
+        <v>44100.03558572193</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>POINT (4.19087118673537 51.5977289297391)</t>
+          <t>POINT (4.2362459507422 51.5464294871925)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>POINT (4.19045226895481 51.5996645039331)</t>
+          <t>POINT (4.2359522832981 51.548647484284)</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2.290677093605146</v>
+        <v>2.595790709855957</v>
       </c>
       <c r="F11" t="n">
-        <v>1774.889172311228</v>
+        <v>2011.936583994549</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8414569232725087</v>
+        <v>0.9575918783590811</v>
       </c>
       <c r="H11" t="n">
-        <v>25.22441673747447</v>
+        <v>28.68937724345811</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -903,32 +901,32 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44100.02224001205</v>
+        <v>44100.03558572193</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44100.02487437565</v>
+        <v>44100.03806398434</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>POINT (4.19045226895481 51.5996645039331)</t>
+          <t>POINT (4.2359522832981 51.548647484284)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>POINT (4.19032195489369 51.6017086380131)</t>
+          <t>POINT (4.23590351148177 51.5505717831532)</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2.399362287652966</v>
+        <v>2.244713064226494</v>
       </c>
       <c r="F12" t="n">
-        <v>1859.101903393073</v>
+        <v>1739.824523415862</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8813813233865395</v>
+        <v>0.828078701608094</v>
       </c>
       <c r="H12" t="n">
-        <v>26.42123344772125</v>
+        <v>24.80917266838098</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -944,32 +942,32 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44100.02487437565</v>
+        <v>44100.03806398434</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44100.02815470932</v>
+        <v>44100.04038316107</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>POINT (4.19032195489369 51.6017086380131)</t>
+          <t>POINT (4.23590351148177 51.5505717831532)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>POINT (4.19044573249358 51.60425485023)</t>
+          <t>POINT (4.23538361411918 51.5523433752533)</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2.987707884881084</v>
+        <v>2.100619492391387</v>
       </c>
       <c r="F13" t="n">
-        <v>2314.970708708307</v>
+        <v>1628.140970609537</v>
       </c>
       <c r="G13" t="n">
-        <v>1.097504092058159</v>
+        <v>0.7749223225573679</v>
       </c>
       <c r="H13" t="n">
-        <v>32.89996175019382</v>
+        <v>23.21661174053494</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -985,32 +983,32 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44100.02815470932</v>
+        <v>44100.04038316107</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44100.0308973893</v>
+        <v>44100.04337659523</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>POINT (4.19044573249358 51.60425485023)</t>
+          <t>POINT (4.23538361411918 51.5523433752533)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>POINT (4.19077174898799 51.6063750103273)</t>
+          <t>POINT (4.23499704828888 51.5546554536382)</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2.4980161833007</v>
+        <v>2.711335464898287</v>
       </c>
       <c r="F14" t="n">
-        <v>1935.542066718164</v>
+        <v>2101.492617540963</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9176208280871099</v>
+        <v>1.00021654738326</v>
       </c>
       <c r="H14" t="n">
-        <v>27.50758777429626</v>
+        <v>29.96640896844057</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1026,32 +1024,32 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44100.0308973893</v>
+        <v>44100.04337659523</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44100.03345011047</v>
+        <v>44100.04658475435</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>POINT (4.19077174898799 51.6063750103273)</t>
+          <t>POINT (4.23499704828888 51.5546554536382)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>POINT (4.19136384668985 51.608322767118)</t>
+          <t>POINT (4.23383845594049 51.5570398210376)</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2.325002859759645</v>
+        <v>2.905824930861236</v>
       </c>
       <c r="F15" t="n">
-        <v>1801.485863249589</v>
+        <v>2252.236847583772</v>
       </c>
       <c r="G15" t="n">
-        <v>0.8540661442670422</v>
+        <v>1.071964062774139</v>
       </c>
       <c r="H15" t="n">
-        <v>25.60240429229896</v>
+        <v>32.1159588764408</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1067,32 +1065,32 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44100.03345011047</v>
+        <v>44100.04658475435</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44100.03635830242</v>
+        <v>44100.04900967324</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>POINT (4.19136384668985 51.608322767118)</t>
+          <t>POINT (4.23383845594049 51.5570398210376)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>POINT (4.19234893854335 51.6104962678729)</t>
+          <t>POINT (4.23280516307828 51.5588093548632)</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2.648763483711804</v>
+        <v>2.196396595777307</v>
       </c>
       <c r="F16" t="n">
-        <v>2052.345850193997</v>
+        <v>1702.375560226871</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9729963150763947</v>
+        <v>0.81025466855187</v>
       </c>
       <c r="H16" t="n">
-        <v>29.16758286403765</v>
+        <v>24.27516604461634</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1108,32 +1106,32 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44100.03635830242</v>
+        <v>44100.04900967324</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44100.03926704481</v>
+        <v>44100.05161956345</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>POINT (4.19234893854335 51.6104962678729)</t>
+          <t>POINT (4.23280516307828 51.5588093548632)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>POINT (4.193649745564273 51.61260489647889)</t>
+          <t>POINT (4.23135933316239 51.5606247189843)</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2.649264810984627</v>
+        <v>2.363936372596425</v>
       </c>
       <c r="F17" t="n">
-        <v>2052.734294418995</v>
+        <v>1832.231717464746</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9731804723822077</v>
+        <v>0.8720603954194192</v>
       </c>
       <c r="H17" t="n">
-        <v>29.17310336195954</v>
+        <v>26.12686074979695</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1149,32 +1147,32 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44100.03926704481</v>
+        <v>44100.05161956345</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44100.03938444692</v>
+        <v>44100.05537797155</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>POINT (4.193649745564273 51.61260489647889)</t>
+          <t>POINT (4.23135933316239 51.5606247189843)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>POINT (4.193702248646781 51.61269000480002)</t>
+          <t>POINT (4.22894307117378 51.5631248020868)</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.1069291317042259</v>
+        <v>3.404218916743891</v>
       </c>
       <c r="F18" t="n">
-        <v>82.8520784017287</v>
+        <v>2638.530353289053</v>
       </c>
       <c r="G18" t="n">
-        <v>0.03927932879382383</v>
+        <v>1.255822503655332</v>
       </c>
       <c r="H18" t="n">
-        <v>1.177479358057499</v>
+        <v>37.62434328272229</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1182,38 +1180,40 @@
       <c r="J18" t="n">
         <v>10</v>
       </c>
-      <c r="K18" t="n">
-        <v>4.3</v>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44100.03938444692</v>
+        <v>44100.05537797155</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44100.04191849671</v>
+        <v>44100.05787677329</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>POINT (4.193702248646781 51.61269000480002)</t>
+          <t>POINT (4.22894307117378 51.5631248020868)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>POINT (4.19483549713345 51.614527018391)</t>
+          <t>POINT (4.22710959891667 51.5646931283473)</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>2.307997083894028</v>
+        <v>2.263316795144454</v>
       </c>
       <c r="F19" t="n">
-        <v>1788.309249400833</v>
+        <v>1754.243839511658</v>
       </c>
       <c r="G19" t="n">
-        <v>0.8478192453541343</v>
+        <v>0.8349416513553363</v>
       </c>
       <c r="H19" t="n">
-        <v>25.41514053995393</v>
+        <v>25.01478610287554</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -1229,32 +1229,32 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44100.04191849671</v>
+        <v>44100.05787677329</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44100.0453304208</v>
+        <v>44100.05825139008</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>POINT (4.19483549713345 51.614527018391)</t>
+          <t>POINT (4.22710959891667 51.5646931283473)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>POINT (4.19679859918884 51.6168778883867)</t>
+          <t>POINT (4.22681457589646 51.5649185661967)</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>3.107559632333117</v>
+        <v>0.3393132159399787</v>
       </c>
       <c r="F20" t="n">
-        <v>2407.835639133378</v>
+        <v>262.9937267019764</v>
       </c>
       <c r="G20" t="n">
-        <v>1.141530412270393</v>
+        <v>0.1251732576872993</v>
       </c>
       <c r="H20" t="n">
-        <v>34.21974202283036</v>
+        <v>3.750180940651032</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1270,32 +1270,32 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44100.0453304208</v>
+        <v>44100.05825139008</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44100.04754763832</v>
+        <v>44100.05868165311</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>POINT (4.19679859918884 51.6168778883867)</t>
+          <t>POINT (4.22681457589646 51.5649185661967)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>POINT (4.19825019008788 51.6183435014205)</t>
+          <t>POINT (4.22648005518784 51.565179667521)</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2.01942818754376</v>
+        <v>0.3897154092605516</v>
       </c>
       <c r="F21" t="n">
-        <v>1564.71692771219</v>
+        <v>302.0592863523562</v>
       </c>
       <c r="G21" t="n">
-        <v>0.7418163973950417</v>
+        <v>0.1437667181754688</v>
       </c>
       <c r="H21" t="n">
-        <v>22.2374852871125</v>
+        <v>4.307239550626561</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -1311,32 +1311,32 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44100.04754763832</v>
+        <v>44100.05868165311</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44100.05081235724</v>
+        <v>44100.06084702971</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>POINT (4.19825019008788 51.6183435014205)</t>
+          <t>POINT (4.22648005518784 51.565179667521)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>POINT (4.20060308876194 51.6204128525436)</t>
+          <t>POINT (4.22475858224584 51.5664744891401)</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2.97348606097947</v>
+        <v>1.961313347826133</v>
       </c>
       <c r="F22" t="n">
-        <v>2303.951188991692</v>
+        <v>1520.168040601867</v>
       </c>
       <c r="G22" t="n">
-        <v>1.092279849350757</v>
+        <v>0.7235320343655131</v>
       </c>
       <c r="H22" t="n">
-        <v>32.74335423984017</v>
+        <v>21.67696275450049</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1344,40 +1344,38 @@
       <c r="J22" t="n">
         <v>10</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
+      <c r="K22" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44100.05081235724</v>
+        <v>44100.06084702971</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44100.05384891604</v>
+        <v>44100.0756526418</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>POINT (4.20060308876194 51.6204128525436)</t>
+          <t>POINT (4.22475858224584 51.5664744891401)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>POINT (4.20307825061863 51.6221979794345)</t>
+          <t>POINT (4.2130453756528 51.5753578449578)</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>2.765679228587873</v>
+        <v>13.41034378627525</v>
       </c>
       <c r="F23" t="n">
-        <v>2142.935872795703</v>
+        <v>10394.04338945898</v>
       </c>
       <c r="G23" t="n">
-        <v>1.015944124450912</v>
+        <v>4.947100030485215</v>
       </c>
       <c r="H23" t="n">
-        <v>30.45503253778886</v>
+        <v>148.2147272100811</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1393,32 +1391,32 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44100.05384891604</v>
+        <v>44100.0756526418</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44100.05648473466</v>
+        <v>44100.08756776695</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>POINT (4.20307825061863 51.6221979794345)</t>
+          <t>POINT (4.2130453756528 51.5753578449578)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>POINT (4.20540322490335 51.6236455127064)</t>
+          <t>POINT (4.20361777418235 51.58250715914)</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2.400687514315178</v>
+        <v>10.7922538963779</v>
       </c>
       <c r="F24" t="n">
-        <v>1860.128730968863</v>
+        <v>8364.823233182729</v>
       </c>
       <c r="G24" t="n">
-        <v>0.8818681317871047</v>
+        <v>3.98128194375954</v>
       </c>
       <c r="H24" t="n">
-        <v>26.43582653985767</v>
+        <v>119.2788934143756</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -1434,32 +1432,32 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44100.05648473466</v>
+        <v>44100.08756776695</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44100.05944331045</v>
+        <v>44100.09027698619</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>POINT (4.20540322490335 51.6236455127064)</t>
+          <t>POINT (4.20361777418235 51.58250715914)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>POINT (4.20831515432923 51.6250574284908)</t>
+          <t>POINT (4.201416987493968 51.58410292465058)</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>2.694652769130375</v>
+        <v>2.453904717551025</v>
       </c>
       <c r="F25" t="n">
-        <v>2087.902322154853</v>
+        <v>1901.964074505773</v>
       </c>
       <c r="G25" t="n">
-        <v>0.989853277262166</v>
+        <v>0.9052498801902094</v>
       </c>
       <c r="H25" t="n">
-        <v>29.67290527211757</v>
+        <v>27.12121509942025</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -1475,32 +1473,32 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44100.05944331045</v>
+        <v>44100.09027698619</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44100.06273990944</v>
+        <v>44100.09037664615</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>POINT (4.20831515432923 51.6250574284908)</t>
+          <t>POINT (4.201416987493968 51.58410292465058)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>POINT (4.21163878092211 51.6265655036704)</t>
+          <t>POINT (4.201336029861413 51.58416162611335)</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3.002522241907305</v>
+        <v>0.09026808454713277</v>
       </c>
       <c r="F26" t="n">
-        <v>2326.449341834585</v>
+        <v>69.96467818594724</v>
       </c>
       <c r="G26" t="n">
-        <v>1.102945995623491</v>
+        <v>0.03330005929124567</v>
       </c>
       <c r="H26" t="n">
-        <v>33.06309409689923</v>
+        <v>0.9976671533694728</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1508,40 +1506,38 @@
       <c r="J26" t="n">
         <v>10</v>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
+      <c r="K26" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44100.06273990944</v>
+        <v>44100.09037664615</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44100.06609599468</v>
+        <v>44100.09059161645</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>POINT (4.21163878092211 51.6265655036704)</t>
+          <t>POINT (4.201336029861413 51.58416162611335)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>POINT (4.21531323447367 51.6278153710409)</t>
+          <t>POINT (4.20116140102169 51.5842882475079)</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>3.056701944362318</v>
+        <v>0.1947116840860167</v>
       </c>
       <c r="F27" t="n">
-        <v>2368.429491528284</v>
+        <v>150.9164659865972</v>
       </c>
       <c r="G27" t="n">
-        <v>1.122848358175291</v>
+        <v>0.07182949129925477</v>
       </c>
       <c r="H27" t="n">
-        <v>33.65970869804375</v>
+        <v>2.152005902816833</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
@@ -1557,32 +1553,32 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44100.06609599468</v>
+        <v>44100.09059161645</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44100.07683285182</v>
+        <v>44100.09294389399</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>POINT (4.21531323447367 51.6278153710409)</t>
+          <t>POINT (4.20116140102169 51.5842882475079)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>POINT (4.22766582279304 51.6310429998208)</t>
+          <t>POINT (4.19934887369148 51.5857241535032)</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>9.779063952648158</v>
+        <v>2.130600908297478</v>
       </c>
       <c r="F28" t="n">
-        <v>7577.128515043341</v>
+        <v>1651.378863984405</v>
       </c>
       <c r="G28" t="n">
-        <v>3.592239642981919</v>
+        <v>0.785982521586636</v>
       </c>
       <c r="H28" t="n">
-        <v>107.6848348038795</v>
+        <v>23.54797442985325</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -1598,32 +1594,32 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44100.07683285182</v>
+        <v>44100.09294389399</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44100.08516529221</v>
+        <v>44100.09531342501</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>POINT (4.22766582279304 51.6310429998208)</t>
+          <t>POINT (4.19934887369148 51.5857241535032)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>POINT (4.23716835589874 51.6336694704785)</t>
+          <t>POINT (4.19763109913537 51.5872210992283)</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>7.58913585367172</v>
+        <v>2.146228430631858</v>
       </c>
       <c r="F29" t="n">
-        <v>5880.302855159734</v>
+        <v>1663.491390421103</v>
       </c>
       <c r="G29" t="n">
-        <v>2.787791838003799</v>
+        <v>0.79174754203593</v>
       </c>
       <c r="H29" t="n">
-        <v>83.56984315567365</v>
+        <v>23.72069399140515</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -1639,32 +1635,32 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44100.08516529221</v>
+        <v>44100.09531342501</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44100.08890978585</v>
+        <v>44100.09837348539</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>POINT (4.23716835589874 51.6336694704785)</t>
+          <t>POINT (4.19763109913537 51.5872210992283)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>POINT (4.24161396068552 51.634565032025)</t>
+          <t>POINT (4.19562926259692 51.5892439548483)</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>3.410461948001152</v>
+        <v>2.771682892637499</v>
       </c>
       <c r="F30" t="n">
-        <v>2642.533948109791</v>
+        <v>2148.266495409977</v>
       </c>
       <c r="G30" t="n">
-        <v>1.25279849578944</v>
+        <v>1.022478822449302</v>
       </c>
       <c r="H30" t="n">
-        <v>37.55523363419607</v>
+        <v>30.63338497558098</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -1680,32 +1676,32 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44100.08890978585</v>
+        <v>44100.09837348539</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>44100.09010144613</v>
+        <v>44100.10191112708</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>POINT (4.24161396068552 51.634565032025)</t>
+          <t>POINT (4.19562926259692 51.5892439548483)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>POINT (4.24290239708188 51.6350271044531)</t>
+          <t>POINT (4.19369271232264 51.5917121585537)</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.085356917861739</v>
+        <v>3.204257344887606</v>
       </c>
       <c r="F31" t="n">
-        <v>840.9689200681373</v>
+        <v>2483.544822126127</v>
       </c>
       <c r="G31" t="n">
-        <v>0.3986948206209332</v>
+        <v>1.182056318505846</v>
       </c>
       <c r="H31" t="n">
-        <v>11.95170427386437</v>
+        <v>35.41431418783986</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -1721,32 +1717,32 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44100.09010144613</v>
+        <v>44100.10191112708</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44100.09965610482</v>
+        <v>44100.10472595942</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>POINT (4.24290239708188 51.6350271044531)</t>
+          <t>POINT (4.19369271232264 51.5917121585537)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>POINT (4.25322483053807 51.6387412893827)</t>
+          <t>POINT (4.19244257593752 51.5937546589974)</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>8.70232482139755</v>
+        <v>2.549564931087124</v>
       </c>
       <c r="F32" t="n">
-        <v>6742.836929010628</v>
+        <v>1976.108065563424</v>
       </c>
       <c r="G32" t="n">
-        <v>3.196710478521697</v>
+        <v>0.940539105469305</v>
       </c>
       <c r="H32" t="n">
-        <v>95.82802764033116</v>
+        <v>28.17847750961459</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -1754,38 +1750,40 @@
       <c r="J32" t="n">
         <v>10</v>
       </c>
-      <c r="K32" t="n">
-        <v>4.3</v>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44100.09965610482</v>
+        <v>44100.10472595942</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44100.101136593</v>
+        <v>44100.10705784795</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>POINT (4.25322483053807 51.6387412893827)</t>
+          <t>POINT (4.19244257593752 51.5937546589974)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>POINT (4.25487324647157 51.6392606516986)</t>
+          <t>POINT (4.19160568283927 51.5954888733602)</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1.348419590013013</v>
+        <v>2.112133336414411</v>
       </c>
       <c r="F33" t="n">
-        <v>1044.798211297135</v>
+        <v>1637.065081507072</v>
       </c>
       <c r="G33" t="n">
-        <v>0.4953282165931814</v>
+        <v>0.7791698007669881</v>
       </c>
       <c r="H33" t="n">
-        <v>14.84849076822036</v>
+        <v>23.34386585163047</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -1793,36 +1791,40 @@
       <c r="J33" t="n">
         <v>10</v>
       </c>
-      <c r="K33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44100.101136593</v>
+        <v>44100.10705784795</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44100.11543891381</v>
+        <v>44100.11000196481</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>POINT (4.25487324647157 51.6392606516986)</t>
+          <t>POINT (4.19160568283927 51.5954888733602)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>POINT (4.2707705563819 51.6443125466199)</t>
+          <t>POINT (4.19087118673537 51.5977289297391)</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>13.02646650128897</v>
+        <v>2.66666579293431</v>
       </c>
       <c r="F34" t="n">
-        <v>10093.31887539667</v>
+        <v>2066.870200992897</v>
       </c>
       <c r="G34" t="n">
-        <v>4.785139927422893</v>
+        <v>0.9837378247436269</v>
       </c>
       <c r="H34" t="n">
-        <v>143.4444953043636</v>
+        <v>29.47270773631998</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -1830,36 +1832,38 @@
       <c r="J34" t="n">
         <v>10</v>
       </c>
-      <c r="K34" t="inlineStr"/>
+      <c r="K34" t="n">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44100.11543891381</v>
+        <v>44100.11000196481</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44100.13161045006</v>
+        <v>44100.11251699823</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>POINT (4.2707705563819 51.6443125466199)</t>
+          <t>POINT (4.19087118673537 51.5977289297391)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>POINT (4.28858704214208 51.6502162851357)</t>
+          <t>POINT (4.19045226895481 51.5996645039331)</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>14.72893651367311</v>
+        <v>2.278018805034489</v>
       </c>
       <c r="F35" t="n">
-        <v>11412.44656900767</v>
+        <v>1765.639022971873</v>
       </c>
       <c r="G35" t="n">
-        <v>5.410524964629227</v>
+        <v>0.8403652488675005</v>
       </c>
       <c r="H35" t="n">
-        <v>162.1917090503646</v>
+        <v>25.17727665901985</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -1867,36 +1871,40 @@
       <c r="J35" t="n">
         <v>10</v>
       </c>
-      <c r="K35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44100.13161045006</v>
+        <v>44100.11251699823</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44100.13602087353</v>
+        <v>44100.11515136183</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>POINT (4.28858704214208 51.6502162851357)</t>
+          <t>POINT (4.19045226895481 51.5996645039331)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>POINT (4.29344689234686 51.6518259266097)</t>
+          <t>POINT (4.19032195489369 51.6017086380131)</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>4.016986780111385</v>
+        <v>2.386103413238025</v>
       </c>
       <c r="F36" t="n">
-        <v>3112.488600482985</v>
+        <v>1849.412871454028</v>
       </c>
       <c r="G36" t="n">
-        <v>1.475599221555417</v>
+        <v>0.8802378564399984</v>
       </c>
       <c r="H36" t="n">
-        <v>44.23414755235805</v>
+        <v>26.37185683895936</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -1912,32 +1920,32 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44100.13602087353</v>
+        <v>44100.11515136183</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44100.14181761008</v>
+        <v>44100.11843169551</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>POINT (4.29344689234686 51.6518259266097)</t>
+          <t>POINT (4.19032195489369 51.6017086380131)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>POINT (4.29994100636514 51.6538121920118)</t>
+          <t>POINT (4.19044573249358 51.60425485023)</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>5.279632271470039</v>
+        <v>2.971197821522766</v>
       </c>
       <c r="F37" t="n">
-        <v>4090.826323097535</v>
+        <v>2302.905844072704</v>
       </c>
       <c r="G37" t="n">
-        <v>1.939419195491041</v>
+        <v>1.096080240238518</v>
       </c>
       <c r="H37" t="n">
-        <v>58.1381133893109</v>
+        <v>32.83847765317583</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -1953,32 +1961,32 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44100.14181761008</v>
+        <v>44100.11843169551</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44100.14694563681</v>
+        <v>44100.12117437548</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>POINT (4.29994100636514 51.6538121920118)</t>
+          <t>POINT (4.19044573249358 51.60425485023)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>POINT (4.30598376599959 51.6551275816558)</t>
+          <t>POINT (4.19077174898799 51.6063750103273)</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>4.670575441662757</v>
+        <v>2.484212147502378</v>
       </c>
       <c r="F38" t="n">
-        <v>3618.90979875781</v>
+        <v>1925.454653597704</v>
       </c>
       <c r="G38" t="n">
-        <v>1.715688366474555</v>
+        <v>0.9164303455349386</v>
       </c>
       <c r="H38" t="n">
-        <v>51.43131769548883</v>
+        <v>27.45618096152232</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -1994,32 +2002,32 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44100.14694563681</v>
+        <v>44100.12117437548</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>44100.15549219927</v>
+        <v>44100.12372709664</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>POINT (4.30598376599959 51.6551275816558)</t>
+          <t>POINT (4.19077174898799 51.6063750103273)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>POINT (4.31624886074167 51.6569393362889)</t>
+          <t>POINT (4.19136384668985 51.608322767118)</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>7.784156930463684</v>
+        <v>2.312154887041795</v>
       </c>
       <c r="F39" t="n">
-        <v>6031.411362972145</v>
+        <v>1792.09710065362</v>
       </c>
       <c r="G39" t="n">
-        <v>2.859430846061891</v>
+        <v>0.8529581111913408</v>
       </c>
       <c r="H39" t="n">
-        <v>85.71737102627239</v>
+        <v>25.55455782204733</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
@@ -2035,32 +2043,32 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44100.15549219927</v>
+        <v>44100.12372709664</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>44100.16385886945</v>
+        <v>44100.1266352886</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>POINT (4.31624886074167 51.6569393362889)</t>
+          <t>POINT (4.19136384668985 51.608322767118)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>POINT (4.32633341388214 51.65863405384)</t>
+          <t>POINT (4.19234893854335 51.6104962678729)</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>7.620312128256028</v>
+        <v>2.634126418432069</v>
       </c>
       <c r="F40" t="n">
-        <v>5904.459220265678</v>
+        <v>2041.649693902807</v>
       </c>
       <c r="G40" t="n">
-        <v>2.799244125317994</v>
+        <v>0.9717339907035514</v>
       </c>
       <c r="H40" t="n">
-        <v>83.91314922355274</v>
+        <v>29.11307381426246</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -2068,36 +2076,40 @@
       <c r="J40" t="n">
         <v>10</v>
       </c>
-      <c r="K40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44100.16385886945</v>
+        <v>44100.1266352886</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44100.17653906924</v>
+        <v>44100.129544031</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>POINT (4.32633341388214 51.65863405384)</t>
+          <t>POINT (4.19234893854335 51.6104962678729)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>POINT (4.34215442577575 51.6590038262397)</t>
+          <t>POINT (4.193649745564273 51.61260489647889)</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>11.54904857708627</v>
+        <v>2.634624983812692</v>
       </c>
       <c r="F41" t="n">
-        <v>8948.568668641212</v>
+        <v>2042.036120316672</v>
       </c>
       <c r="G41" t="n">
-        <v>4.242425485688794</v>
+        <v>0.9719179127811532</v>
       </c>
       <c r="H41" t="n">
-        <v>127.175504141092</v>
+        <v>29.11858410357042</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -2113,32 +2125,32 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44100.17653906924</v>
+        <v>44100.129544031</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>44100.18692711704</v>
+        <v>44100.1296614331</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>POINT (4.34215442577575 51.6590038262397)</t>
+          <t>POINT (4.193649745564273 51.61260489647889)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>POINT (4.35443838138702 51.6615938492316)</t>
+          <t>POINT (4.193702248646781 51.61269000480002)</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>9.461370533048607</v>
+        <v>0.1063382329703281</v>
       </c>
       <c r="F42" t="n">
-        <v>7330.969590248839</v>
+        <v>82.42027380917426</v>
       </c>
       <c r="G42" t="n">
-        <v>3.475538198156234</v>
+        <v>0.03922836576094399</v>
       </c>
       <c r="H42" t="n">
-        <v>104.1864669158243</v>
+        <v>1.175278749385503</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -2146,40 +2158,38 @@
       <c r="J42" t="n">
         <v>10</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>'NoneType' object is not subscriptable</t>
-        </is>
+      <c r="K42" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44100.18692711704</v>
+        <v>44100.1296614331</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44100.1939491187</v>
+        <v>44100.1321954829</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>POINT (4.35443838138702 51.6615938492316)</t>
+          <t>POINT (4.193702248646781 51.61269000480002)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>POINT (4.36248182981987 51.6637647088662)</t>
+          <t>POINT (4.19483549713345 51.614527018391)</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>6.395596259989223</v>
+        <v>2.295243093521373</v>
       </c>
       <c r="F43" t="n">
-        <v>4955.510571034728</v>
+        <v>1778.989165643911</v>
       </c>
       <c r="G43" t="n">
-        <v>2.349357212129136</v>
+        <v>0.8467193204311094</v>
       </c>
       <c r="H43" t="n">
-        <v>70.426855785806</v>
+        <v>25.36764414072094</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -2187,36 +2197,40 @@
       <c r="J43" t="n">
         <v>10</v>
       </c>
-      <c r="K43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44100.1939491187</v>
+        <v>44100.1321954829</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>44100.20404210483</v>
+        <v>44100.13560740698</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>POINT (4.36248182981987 51.6637647088662)</t>
+          <t>POINT (4.19483549713345 51.614527018391)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>POINT (4.37376673844804 51.6672551204272)</t>
+          <t>POINT (4.19679859918884 51.6168778883867)</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>9.192630158618535</v>
+        <v>3.090387259876907</v>
       </c>
       <c r="F44" t="n">
-        <v>7122.741035386243</v>
+        <v>2395.286786192181</v>
       </c>
       <c r="G44" t="n">
-        <v>3.376819155642483</v>
+        <v>1.140049438871568</v>
       </c>
       <c r="H44" t="n">
-        <v>101.2271588415937</v>
+        <v>34.15579138192415</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -2232,32 +2246,32 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44100.20404210483</v>
+        <v>44100.13560740698</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>44100.20741604888</v>
+        <v>44100.1378246245</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>POINT (4.37376673844804 51.6672551204272)</t>
+          <t>POINT (4.19679859918884 51.6168778883867)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>POINT (4.37711458868196 51.668845982073)</t>
+          <t>POINT (4.19825019008788 51.6183435014205)</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3.072967649011126</v>
+        <v>2.008268828699037</v>
       </c>
       <c r="F45" t="n">
-        <v>2381.032674687639</v>
+        <v>1556.562134109004</v>
       </c>
       <c r="G45" t="n">
-        <v>1.128823399023705</v>
+        <v>0.740853996094944</v>
       </c>
       <c r="H45" t="n">
-        <v>33.83882294273558</v>
+        <v>22.19592736309585</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -2273,32 +2287,32 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44100.20741604888</v>
+        <v>44100.1378246245</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44100.21109039142</v>
+        <v>44100.14108934343</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>POINT (4.37711458868196 51.668845982073)</t>
+          <t>POINT (4.19825019008788 51.6183435014205)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>POINT (4.38041227511533 51.6708301366592)</t>
+          <t>POINT (4.20060308876194 51.6204128525436)</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3.34656876532737</v>
+        <v>2.957054587309031</v>
       </c>
       <c r="F46" t="n">
-        <v>2593.027486271129</v>
+        <v>2291.943754419982</v>
       </c>
       <c r="G46" t="n">
-        <v>1.229327985211636</v>
+        <v>1.090862775238191</v>
       </c>
       <c r="H46" t="n">
-        <v>36.85165639403699</v>
+        <v>32.68216281425224</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -2314,32 +2328,32 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44100.21109039142</v>
+        <v>44100.14108934343</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>44100.21669247686</v>
+        <v>44100.14412590223</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>POINT (4.38041227511533 51.6708301366592)</t>
+          <t>POINT (4.20060308876194 51.6204128525436)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>POINT (4.38419738555173 51.6744888976717)</t>
+          <t>POINT (4.20307825061863 51.6221979794345)</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>5.102345228503392</v>
+        <v>2.750396087001112</v>
       </c>
       <c r="F47" t="n">
-        <v>3953.45870636587</v>
+        <v>2131.767590909245</v>
       </c>
       <c r="G47" t="n">
-        <v>1.874294603836077</v>
+        <v>1.014626081403085</v>
       </c>
       <c r="H47" t="n">
-        <v>56.18586866542668</v>
+        <v>30.39811747251348</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
@@ -2355,32 +2369,32 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44100.21669247686</v>
+        <v>44100.14412590223</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44100.22303713625</v>
+        <v>44100.14676172085</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>POINT (4.38419738555173 51.6744888976717)</t>
+          <t>POINT (4.20307825061863 51.6221979794345)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>POINT (4.38803424793866 51.6787998977028)</t>
+          <t>POINT (4.20540322490335 51.6236455127064)</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>5.778677044202638</v>
+        <v>2.38742131666567</v>
       </c>
       <c r="F48" t="n">
-        <v>4477.502020979587</v>
+        <v>1850.434347515917</v>
       </c>
       <c r="G48" t="n">
-        <v>2.12273821557429</v>
+        <v>0.8807240332742555</v>
       </c>
       <c r="H48" t="n">
-        <v>63.63348127918758</v>
+        <v>26.3864226590965</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -2396,32 +2410,32 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44100.22303713625</v>
+        <v>44100.14676172085</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>44100.22719413898</v>
+        <v>44100.14972029664</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>POINT (4.38803424793866 51.6787998977028)</t>
+          <t>POINT (4.20540322490335 51.6236455127064)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>POINT (4.39198470467551 51.6808950327794)</t>
+          <t>POINT (4.20831515432923 51.6250574284908)</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>3.786172715661048</v>
+        <v>2.679762119715252</v>
       </c>
       <c r="F49" t="n">
-        <v>2933.646552034988</v>
+        <v>2077.020857163065</v>
       </c>
       <c r="G49" t="n">
-        <v>1.390812023612791</v>
+        <v>0.9885690833789789</v>
       </c>
       <c r="H49" t="n">
-        <v>41.6924754164524</v>
+        <v>29.61745186427571</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
@@ -2429,36 +2443,40 @@
       <c r="J49" t="n">
         <v>10</v>
       </c>
-      <c r="K49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>44100.22719413898</v>
+        <v>44100.14972029664</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>44100.22784076325</v>
+        <v>44100.15301689564</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>POINT (4.39198470467551 51.6808950327794)</t>
+          <t>POINT (4.20831515432923 51.6250574284908)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>POINT (4.3925552967856 51.6812504548851)</t>
+          <t>POINT (4.21163878092211 51.6265655036704)</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.5889414403448433</v>
+        <v>2.985930305999536</v>
       </c>
       <c r="F50" t="n">
-        <v>456.3304834146991</v>
+        <v>2314.32464769304</v>
       </c>
       <c r="G50" t="n">
-        <v>0.2163416454409889</v>
+        <v>1.101515080019003</v>
       </c>
       <c r="H50" t="n">
-        <v>6.485289588212888</v>
+        <v>33.00130502623567</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -2474,32 +2492,32 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>44100.22784076325</v>
+        <v>44100.15301689564</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>44100.24168224123</v>
+        <v>44100.15637298085</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>POINT (4.3925552967856 51.6812504548851)</t>
+          <t>POINT (4.21163878092211 51.6265655036704)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>POINT (4.40615183993005 51.6878914989466)</t>
+          <t>POINT (4.21531323447367 51.6278153710409)</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>12.60673365769716</v>
+        <v>3.039810603001111</v>
       </c>
       <c r="F51" t="n">
-        <v>9768.096572670598</v>
+        <v>2356.086003915543</v>
       </c>
       <c r="G51" t="n">
-        <v>4.630955338479966</v>
+        <v>1.121391618394961</v>
       </c>
       <c r="H51" t="n">
-        <v>138.8224924186018</v>
+        <v>33.59680455203917</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -2507,38 +2525,40 @@
       <c r="J51" t="n">
         <v>10</v>
       </c>
-      <c r="K51" t="n">
-        <v>4.75</v>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>44100.24168224123</v>
+        <v>44100.15637298085</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>44100.24323851532</v>
+        <v>44100.167109838</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>POINT (4.40615183993005 51.6878914989466)</t>
+          <t>POINT (4.21531323447367 51.6278153710409)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>POINT (4.407623317192122 51.68868147089958)</t>
+          <t>POINT (4.22766582279304 51.6310429998208)</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1.417444949473549</v>
+        <v>9.725024851661356</v>
       </c>
       <c r="F52" t="n">
-        <v>1098.281246244763</v>
+        <v>7537.638995870889</v>
       </c>
       <c r="G52" t="n">
-        <v>0.520683979879373</v>
+        <v>3.58757922281072</v>
       </c>
       <c r="H52" t="n">
-        <v>15.60858236982994</v>
+        <v>107.4835909076762</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
@@ -2554,32 +2574,32 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>44100.24323851532</v>
+        <v>44100.167109838</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>44100.24333169821</v>
+        <v>44100.17544227839</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>POINT (4.407623317192122 51.68868147089958)</t>
+          <t>POINT (4.22766582279304 51.6310429998208)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>POINT (4.407711423268813 51.68872877120878)</t>
+          <t>POINT (4.23716835589874 51.6336694704785)</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0.08487039924488325</v>
+        <v>7.547198293948414</v>
       </c>
       <c r="F53" t="n">
-        <v>65.76027375458418</v>
+        <v>5849.656637171157</v>
       </c>
       <c r="G53" t="n">
-        <v>0.03117627787643261</v>
+        <v>2.784175074479729</v>
       </c>
       <c r="H53" t="n">
-        <v>0.9345735983393422</v>
+        <v>83.41366591061696</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
@@ -2587,46 +2607,1002 @@
       <c r="J53" t="n">
         <v>10</v>
       </c>
-      <c r="K53" t="n">
-        <v>4.75</v>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>44100.24333169821</v>
+        <v>44100.17544227839</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>44100.24446582665</v>
+        <v>44100.17918677202</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>POINT (4.23716835589874 51.6336694704785)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>POINT (4.24161396068552 51.634565032025)</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>3.391615737503959</v>
+      </c>
+      <c r="F54" t="n">
+        <v>2628.761924201857</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1.251173167870853</v>
+      </c>
+      <c r="H54" t="n">
+        <v>37.48504954972244</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>10</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>44100.17918677202</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>44100.18037843231</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>POINT (4.24161396068552 51.634565032025)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>POINT (4.24290239708188 51.6350271044531)</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>1.079359236279721</v>
+      </c>
+      <c r="F55" t="n">
+        <v>836.5860647372665</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.3981775707816131</v>
+      </c>
+      <c r="H55" t="n">
+        <v>11.9293686541055</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>10</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>44100.18037843231</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>44100.18993309102</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>POINT (4.24290239708188 51.6350271044531)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>POINT (4.25322483053807 51.6387412893827)</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>8.654235788577003</v>
+      </c>
+      <c r="F56" t="n">
+        <v>6707.695471736624</v>
+      </c>
+      <c r="G56" t="n">
+        <v>3.192563204892026</v>
+      </c>
+      <c r="H56" t="n">
+        <v>95.64894212627563</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>10</v>
+      </c>
+      <c r="K56" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>44100.18993309102</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>44100.19141357918</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>POINT (4.25322483053807 51.6387412893827)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>POINT (4.25487324647157 51.6392606516986)</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>1.3409682157848</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1039.35305759986</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.4946855949702831</v>
+      </c>
+      <c r="H57" t="n">
+        <v>14.82074145886783</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>10</v>
+      </c>
+      <c r="K57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>44100.19141357918</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>44100.2057159</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>POINT (4.25487324647157 51.6392606516986)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>POINT (4.2707705563819 51.6443125466199)</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>12.95448226440027</v>
+      </c>
+      <c r="F58" t="n">
+        <v>10040.71580047999</v>
+      </c>
+      <c r="G58" t="n">
+        <v>4.778931892436323</v>
+      </c>
+      <c r="H58" t="n">
+        <v>143.1764230403344</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>10</v>
+      </c>
+      <c r="K58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>44100.2057159</v>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>44100.22188743624</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>POINT (4.2707705563819 51.6443125466199)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>POINT (4.28858704214208 51.6502162851357)</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>14.6475444117582</v>
+      </c>
+      <c r="F59" t="n">
+        <v>11352.96861812634</v>
+      </c>
+      <c r="G59" t="n">
+        <v>5.403505574099802</v>
+      </c>
+      <c r="H59" t="n">
+        <v>161.888601345715</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>10</v>
+      </c>
+      <c r="K59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>44100.22188743624</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>44100.22629785971</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>POINT (4.28858704214208 51.6502162851357)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>POINT (4.29344689234686 51.6518259266097)</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>3.994788913779562</v>
+      </c>
+      <c r="F60" t="n">
+        <v>3096.267326403964</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1.473684841373745</v>
+      </c>
+      <c r="H60" t="n">
+        <v>44.15148175989943</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>10</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>44100.22629785971</v>
+      </c>
+      <c r="B61" s="2" t="n">
+        <v>44100.23209459627</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>POINT (4.29344689234686 51.6518259266097)</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>POINT (4.29994100636514 51.6538121920118)</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>5.250457035427807</v>
+      </c>
+      <c r="F61" t="n">
+        <v>4069.506278964474</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1.936903078531746</v>
+      </c>
+      <c r="H61" t="n">
+        <v>58.02946365391524</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>10</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>44100.23209459627</v>
+      </c>
+      <c r="B62" s="2" t="n">
+        <v>44100.237222623</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>POINT (4.29994100636514 51.6538121920118)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>POINT (4.30598376599959 51.6551275816558)</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>4.644765844874855</v>
+      </c>
+      <c r="F62" t="n">
+        <v>3600.049222830543</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1.713462504767534</v>
+      </c>
+      <c r="H62" t="n">
+        <v>51.33520166608688</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>10</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>44100.237222623</v>
+      </c>
+      <c r="B63" s="2" t="n">
+        <v>44100.24576918547</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>POINT (4.30598376599959 51.6551275816558)</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>POINT (4.31624886074167 51.6569393362889)</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>7.741141684347074</v>
+      </c>
+      <c r="F63" t="n">
+        <v>5999.977616755024</v>
+      </c>
+      <c r="G63" t="n">
+        <v>2.855721141108403</v>
+      </c>
+      <c r="H63" t="n">
+        <v>85.55718043159065</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>10</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>44100.24576918547</v>
+      </c>
+      <c r="B64" s="2" t="n">
+        <v>44100.25413585563</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>POINT (4.31624886074167 51.6569393362889)</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>POINT (4.32633341388214 51.65863405384)</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>7.578202288474519</v>
+      </c>
+      <c r="F64" t="n">
+        <v>5873.687107202193</v>
+      </c>
+      <c r="G64" t="n">
+        <v>2.795612504080213</v>
+      </c>
+      <c r="H64" t="n">
+        <v>83.75633040026132</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>10</v>
+      </c>
+      <c r="K64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>44100.25413585563</v>
+      </c>
+      <c r="B65" s="2" t="n">
+        <v>44100.26681605543</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>POINT (4.32633341388214 51.65863405384)</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>POINT (4.34215442577575 51.6590038262397)</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>11.48522854226648</v>
+      </c>
+      <c r="F65" t="n">
+        <v>8901.931651322353</v>
+      </c>
+      <c r="G65" t="n">
+        <v>4.236921541835897</v>
+      </c>
+      <c r="H65" t="n">
+        <v>126.9378356338294</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>10</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>44100.26681605543</v>
+      </c>
+      <c r="B66" s="2" t="n">
+        <v>44100.27720410321</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>POINT (4.34215442577575 51.6590038262397)</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>POINT (4.35443838138702 51.6615938492316)</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>9.409086997306403</v>
+      </c>
+      <c r="F66" t="n">
+        <v>7292.762964407382</v>
+      </c>
+      <c r="G66" t="n">
+        <v>3.471029177829576</v>
+      </c>
+      <c r="H66" t="n">
+        <v>103.9917607419435</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>10</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>44100.27720410321</v>
+      </c>
+      <c r="B67" s="2" t="n">
+        <v>44100.28422610489</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>POINT (4.35443838138702 51.6615938492316)</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>POINT (4.36248182981987 51.6637647088662)</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>6.36025419923643</v>
+      </c>
+      <c r="F67" t="n">
+        <v>4929.684068369063</v>
+      </c>
+      <c r="G67" t="n">
+        <v>2.346309255190914</v>
+      </c>
+      <c r="H67" t="n">
+        <v>70.29524045773924</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
+        <v>10</v>
+      </c>
+      <c r="K67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>44100.28422610489</v>
+      </c>
+      <c r="B68" s="2" t="n">
+        <v>44100.29431909101</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>POINT (4.36248182981987 51.6637647088662)</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>POINT (4.37376673844804 51.6672551204272)</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>9.141831690405624</v>
+      </c>
+      <c r="F68" t="n">
+        <v>7085.619635366666</v>
+      </c>
+      <c r="G68" t="n">
+        <v>3.3724382129245</v>
+      </c>
+      <c r="H68" t="n">
+        <v>101.0379831988018</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>10</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>44100.29431909101</v>
+      </c>
+      <c r="B69" s="2" t="n">
+        <v>44100.29769303506</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>POINT (4.37376673844804 51.6672551204272)</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>POINT (4.37711458868196 51.668845982073)</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>3.055986431796625</v>
+      </c>
+      <c r="F69" t="n">
+        <v>2368.62351001766</v>
+      </c>
+      <c r="G69" t="n">
+        <v>1.12735891116606</v>
+      </c>
+      <c r="H69" t="n">
+        <v>33.77558417206779</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>10</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>44100.29769303506</v>
+      </c>
+      <c r="B70" s="2" t="n">
+        <v>44100.30136737761</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>POINT (4.37711458868196 51.668845982073)</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>POINT (4.38041227511533 51.6708301366592)</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>3.328075628509897</v>
+      </c>
+      <c r="F70" t="n">
+        <v>2579.513473869532</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1.227733106943062</v>
+      </c>
+      <c r="H70" t="n">
+        <v>36.7827871708767</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
+        <v>10</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>44100.30136737761</v>
+      </c>
+      <c r="B71" s="2" t="n">
+        <v>44100.30696946305</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>POINT (4.38041227511533 51.6708301366592)</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>POINT (4.38419738555173 51.6744888976717)</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>5.074149680472996</v>
+      </c>
+      <c r="F71" t="n">
+        <v>3932.85457733586</v>
+      </c>
+      <c r="G71" t="n">
+        <v>1.871862976771139</v>
+      </c>
+      <c r="H71" t="n">
+        <v>56.08086732967415</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>10</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>44100.30696946305</v>
+      </c>
+      <c r="B72" s="2" t="n">
+        <v>44100.31331412243</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>POINT (4.38419738555173 51.6744888976717)</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>POINT (4.38803424793866 51.6787998977028)</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>5.746744070232013</v>
+      </c>
+      <c r="F72" t="n">
+        <v>4454.166736159449</v>
+      </c>
+      <c r="G72" t="n">
+        <v>2.119984260874477</v>
+      </c>
+      <c r="H72" t="n">
+        <v>63.51456145755763</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
+        <v>10</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>44100.31331412243</v>
+      </c>
+      <c r="B73" s="2" t="n">
+        <v>44100.31747112516</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>POINT (4.38803424793866 51.6787998977028)</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>POINT (4.39198470467551 51.6808950327794)</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>3.765250327734984</v>
+      </c>
+      <c r="F73" t="n">
+        <v>2918.357344330598</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1.389007642766742</v>
+      </c>
+      <c r="H73" t="n">
+        <v>41.61455955944857</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="n">
+        <v>10</v>
+      </c>
+      <c r="K73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>44100.31747112516</v>
+      </c>
+      <c r="B74" s="2" t="n">
+        <v>44100.31811774945</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>POINT (4.39198470467551 51.6808950327794)</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>POINT (4.3925552967856 51.6812504548851)</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>0.5856869587380954</v>
+      </c>
+      <c r="F74" t="n">
+        <v>453.9522445774287</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.2160609766046871</v>
+      </c>
+      <c r="H74" t="n">
+        <v>6.473169837976949</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
+        <v>10</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>44100.31811774945</v>
+      </c>
+      <c r="B75" s="2" t="n">
+        <v>44100.33195922741</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>POINT (4.3925552967856 51.6812504548851)</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>POINT (4.40615183993005 51.6878914989466)</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>12.5370688473729</v>
+      </c>
+      <c r="F75" t="n">
+        <v>9717.188436935206</v>
+      </c>
+      <c r="G75" t="n">
+        <v>4.624947328696756</v>
+      </c>
+      <c r="H75" t="n">
+        <v>138.5630576435249</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="n">
+        <v>10</v>
+      </c>
+      <c r="K75" t="n">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>44100.33195922741</v>
+      </c>
+      <c r="B76" s="2" t="n">
+        <v>44100.33351550152</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>POINT (4.40615183993005 51.6878914989466)</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>POINT (4.407623317192122 51.68868147089958)</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>1.409612158074054</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1092.557369729288</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.5200084701400303</v>
+      </c>
+      <c r="H76" t="n">
+        <v>15.57941280034951</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="n">
+        <v>10</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>'NoneType' object is not subscriptable</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>44100.33351550152</v>
+      </c>
+      <c r="B77" s="2" t="n">
+        <v>44100.33360868438</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>POINT (4.407623317192122 51.68868147089958)</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
           <t>POINT (4.407711423268813 51.68872877120878)</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E77" t="n">
+        <v>0.08440139705419922</v>
+      </c>
+      <c r="F77" t="n">
+        <v>65.41754606730096</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.0311358274000836</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.9328269375443052</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="n">
+        <v>10</v>
+      </c>
+      <c r="K77" t="n">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>44100.33360868438</v>
+      </c>
+      <c r="B78" s="2" t="n">
+        <v>44100.33474281285</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>POINT (4.407711423268813 51.68872877120878)</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
         <is>
           <t>POINT (4.40878376619477 51.6893044653478)</t>
         </is>
       </c>
-      <c r="E54" t="n">
-        <v>1.032957270478573</v>
-      </c>
-      <c r="F54" t="n">
-        <v>800.3680133779364</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0.3794463428581991</v>
-      </c>
-      <c r="H54" t="n">
-        <v>11.37469122698401</v>
-      </c>
-      <c r="I54" t="n">
-        <v>0</v>
-      </c>
-      <c r="J54" t="n">
-        <v>10</v>
-      </c>
-      <c r="K54" t="n">
+      <c r="E78" t="n">
+        <v>1.027249157683271</v>
+      </c>
+      <c r="F78" t="n">
+        <v>796.1967632933972</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.37895406886805</v>
+      </c>
+      <c r="H78" t="n">
+        <v>11.3534340504944</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="n">
+        <v>10</v>
+      </c>
+      <c r="K78" t="n">
         <v>4.75</v>
       </c>
     </row>

</xml_diff>